<commit_message>
Add Function and Abstraction of SOM tools
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -8,8 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$B$4:$H$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$B$2:$K$65</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">data!$B$4:$H$23</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -17,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
   <si>
     <t>name</t>
   </si>
@@ -325,20 +328,34 @@
     <t>nf = (1)*ga/(2*Se)*(Sut/gm)^2*(-1+(1+(2*gm*Se/(Sut*ga))^2)^(0.5))</t>
   </si>
   <si>
+    <t>0.9*Sut</t>
+  </si>
+  <si>
+    <t>Db</t>
+  </si>
+  <si>
+    <t>σs</t>
+  </si>
+  <si>
+    <t>ηf</t>
+  </si>
+  <si>
+    <t>θp</t>
+  </si>
+  <si>
     <t>(-1)*(1/((ga/Se)+(gm/Sut)))</t>
-  </si>
-  <si>
-    <t>0.9*Sut</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="##0.000E+0"/>
+    <numFmt numFmtId="165" formatCode="##0.00E+0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,6 +386,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -406,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -452,6 +476,20 @@
     <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,7 +797,7 @@
   <dimension ref="B4:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +850,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="6">
-        <v>3.2838474307105938E-3</v>
+        <v>3.6218605889890582E-3</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>5</v>
@@ -842,7 +880,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="6">
-        <v>3.4965858376044989E-2</v>
+        <v>3.4678117394444263E-2</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>5</v>
@@ -869,7 +907,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="8">
-        <v>3.8406174949018066</v>
+        <v>3.1415154578360882</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
@@ -878,7 +916,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>6</v>
@@ -896,7 +934,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="8">
-        <v>77.958128756145143</v>
+        <v>42.823990013566025</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>5</v>
@@ -905,7 +943,7 @@
         <v>35</v>
       </c>
       <c r="G8" s="2">
-        <v>180</v>
+        <v>540</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>15</v>
@@ -1000,7 +1038,7 @@
         <v>48</v>
       </c>
       <c r="D13" s="6">
-        <v>5.0000000000000002E-5</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>7</v>
@@ -1033,7 +1071,7 @@
       <c r="I14" s="17"/>
       <c r="J14" s="20">
         <f>PI()*D5^4/64</f>
-        <v>5.7082342122424748E-12</v>
+        <v>8.4468895846728925E-12</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -1057,7 +1095,7 @@
       <c r="I15" s="17"/>
       <c r="J15" s="20">
         <f>D6/D5</f>
-        <v>10.647832797907638</v>
+        <v>9.574669301151566</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -1081,7 +1119,7 @@
       <c r="I16" s="17"/>
       <c r="J16" s="20">
         <f>(4*J15^2-J15-1)/(4*J15*(J15-1))</f>
-        <v>1.0753040666238485</v>
+        <v>1.0844218490768605</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -1105,7 +1143,7 @@
       <c r="I17" s="17"/>
       <c r="J17" s="20">
         <f>(PI()/180)*(D11*J14)/(PI()*D6*D7)</f>
-        <v>4.8646460803806794E-2</v>
+        <v>8.8735381139592465E-2</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -1131,7 +1169,7 @@
       <c r="I18" s="17"/>
       <c r="J18" s="21">
         <f>J17*D8</f>
-        <v>3.792387054873938</v>
+        <v>3.8000030757718828</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -1149,7 +1187,7 @@
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>22</v>
@@ -1157,7 +1195,7 @@
       <c r="I19" s="17"/>
       <c r="J19" s="21">
         <f>J17*(D8+D12)</f>
-        <v>5.2517808789881419</v>
+        <v>6.4620645099596574</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -1175,7 +1213,7 @@
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="7">
-        <v>1.4800000000000001E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>42</v>
@@ -1183,7 +1221,7 @@
       <c r="I20" s="17"/>
       <c r="J20" s="20">
         <f>(1+D7)*(D5+D13)</f>
-        <v>1.613788019843114E-2</v>
+        <v>1.4999991615425503E-2</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -1201,12 +1239,16 @@
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="7">
-        <v>3.7999999999999999E-2</v>
+        <v>3.8300000000000001E-2</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>41</v>
       </c>
       <c r="I21" s="17"/>
+      <c r="J21" s="20">
+        <f>D6+D5</f>
+        <v>3.829997798343332E-2</v>
+      </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
@@ -1243,7 +1285,7 @@
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>69</v>
@@ -1251,7 +1293,7 @@
       <c r="I23" s="18"/>
       <c r="J23" s="22">
         <f>(J16*32*J19)/(PI()*D5^3)/1000000</f>
-        <v>1624.3854000976967</v>
+        <v>1502.3615673139459</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1382,12 +1424,14 @@
         <v>74</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="5">
+        <v>1</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5" t="s">
         <v>75</v>
@@ -1415,7 +1459,2099 @@
       <c r="I31" s="19"/>
     </row>
   </sheetData>
+  <autoFilter ref="B4:H31"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="B2:K65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="24">
+        <v>3.84529021651753</v>
+      </c>
+      <c r="C3" s="24">
+        <v>6.2074741082912697</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1.49693188215425E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>3.6869863013698601E-2</v>
+      </c>
+      <c r="F3" s="26">
+        <v>1581.7340891706499</v>
+      </c>
+      <c r="G3" s="24">
+        <v>1.00148731081491</v>
+      </c>
+      <c r="H3" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I3" s="6">
+        <v>3.33561643835616E-2</v>
+      </c>
+      <c r="J3" s="25">
+        <v>3.2602739726027399</v>
+      </c>
+      <c r="K3" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="24">
+        <v>3.8381970392376199</v>
+      </c>
+      <c r="C4" s="24">
+        <v>6.1960235514200601</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1.49693188215425E-2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3.69315068493151E-2</v>
+      </c>
+      <c r="F4" s="26">
+        <v>1578.5691304524701</v>
+      </c>
+      <c r="G4" s="24">
+        <v>1.0034952469479299</v>
+      </c>
+      <c r="H4" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I4" s="6">
+        <v>3.34178082191781E-2</v>
+      </c>
+      <c r="J4" s="25">
+        <v>3.2602739726027399</v>
+      </c>
+      <c r="K4" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="24">
+        <v>3.8311299824959799</v>
+      </c>
+      <c r="C5" s="24">
+        <v>6.1846151610839701</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1.49693188215425E-2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3.6993150684931503E-2</v>
+      </c>
+      <c r="F5" s="26">
+        <v>1575.4168114901499</v>
+      </c>
+      <c r="G5" s="24">
+        <v>1.0055031835603101</v>
+      </c>
+      <c r="H5" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I5" s="6">
+        <v>3.3479452054794502E-2</v>
+      </c>
+      <c r="J5" s="25">
+        <v>3.2602739726027399</v>
+      </c>
+      <c r="K5" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="24">
+        <v>3.8352061079114401</v>
+      </c>
+      <c r="C6" s="24">
+        <v>5.8988673797360196</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1.49952148620754E-2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>3.7034246575342503E-2</v>
+      </c>
+      <c r="F6" s="26">
+        <v>1609.53628463168</v>
+      </c>
+      <c r="G6" s="24">
+        <v>1.0003044944994799</v>
+      </c>
+      <c r="H6" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I6" s="6">
+        <v>3.3602739726027397E-2</v>
+      </c>
+      <c r="J6" s="25">
+        <v>3.3698630136986298</v>
+      </c>
+      <c r="K6" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="24">
+        <v>3.82408890227493</v>
+      </c>
+      <c r="C7" s="24">
+        <v>6.1732487047944602</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1.49693188215425E-2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>3.7054794520548003E-2</v>
+      </c>
+      <c r="F7" s="26">
+        <v>1572.2770567064699</v>
+      </c>
+      <c r="G7" s="24">
+        <v>1.00751112065837</v>
+      </c>
+      <c r="H7" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I7" s="6">
+        <v>3.3541095890411002E-2</v>
+      </c>
+      <c r="J7" s="25">
+        <v>3.2602739726027399</v>
+      </c>
+      <c r="K7" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="24">
+        <v>3.82818335003327</v>
+      </c>
+      <c r="C8" s="24">
+        <v>5.8880657914516599</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1.49952148620754E-2</v>
+      </c>
+      <c r="E8" s="6">
+        <v>3.7095890410958898E-2</v>
+      </c>
+      <c r="F8" s="26">
+        <v>1606.3475235994599</v>
+      </c>
+      <c r="G8" s="24">
+        <v>1.00229019930218</v>
+      </c>
+      <c r="H8" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I8" s="6">
+        <v>3.36643835616438E-2</v>
+      </c>
+      <c r="J8" s="25">
+        <v>3.3698630136986298</v>
+      </c>
+      <c r="K8" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="24">
+        <v>3.8170736556136098</v>
+      </c>
+      <c r="C9" s="24">
+        <v>6.1619239517689497</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.49693188215425E-2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3.7116438356164398E-2</v>
+      </c>
+      <c r="F9" s="26">
+        <v>1569.14979112572</v>
+      </c>
+      <c r="G9" s="24">
+        <v>1.00951905824832</v>
+      </c>
+      <c r="H9" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I9" s="6">
+        <v>3.3602739726027397E-2</v>
+      </c>
+      <c r="J9" s="25">
+        <v>3.2602739726027399</v>
+      </c>
+      <c r="K9" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="24">
+        <v>3.82118626430006</v>
+      </c>
+      <c r="C10" s="24">
+        <v>5.8773036890708603</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1.49952148620754E-2</v>
+      </c>
+      <c r="E10" s="6">
+        <v>3.7157534246575301E-2</v>
+      </c>
+      <c r="F10" s="26">
+        <v>1603.17137159868</v>
+      </c>
+      <c r="G10" s="24">
+        <v>1.00427590468482</v>
+      </c>
+      <c r="H10" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I10" s="6">
+        <v>3.37260273972603E-2</v>
+      </c>
+      <c r="J10" s="25">
+        <v>3.3698630136986298</v>
+      </c>
+      <c r="K10" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="24">
+        <v>3.8100841005982402</v>
+      </c>
+      <c r="C11" s="24">
+        <v>6.1506406729152499</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.49693188215425E-2</v>
+      </c>
+      <c r="E11" s="6">
+        <v>3.7178082191780801E-2</v>
+      </c>
+      <c r="F11" s="26">
+        <v>1566.0349403677399</v>
+      </c>
+      <c r="G11" s="24">
+        <v>1.0115269963362401</v>
+      </c>
+      <c r="H11" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I11" s="6">
+        <v>3.36643835616438E-2</v>
+      </c>
+      <c r="J11" s="25">
+        <v>3.2602739726027399</v>
+      </c>
+      <c r="K11" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="24">
+        <v>3.8142147101993702</v>
+      </c>
+      <c r="C12" s="24">
+        <v>5.8665808564737301</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1.49952148620754E-2</v>
+      </c>
+      <c r="E12" s="6">
+        <v>3.7219178082191801E-2</v>
+      </c>
+      <c r="F12" s="26">
+        <v>1600.00775398121</v>
+      </c>
+      <c r="G12" s="24">
+        <v>1.00626161065215</v>
+      </c>
+      <c r="H12" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I12" s="6">
+        <v>3.3787671232876702E-2</v>
+      </c>
+      <c r="J12" s="25">
+        <v>3.3698630136986298</v>
+      </c>
+      <c r="K12" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="24">
+        <v>3.8031200963526302</v>
+      </c>
+      <c r="C13" s="24">
+        <v>6.1393986408160997</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1.49693188215425E-2</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3.72397260273973E-2</v>
+      </c>
+      <c r="F13" s="26">
+        <v>1562.9324306419899</v>
+      </c>
+      <c r="G13" s="24">
+        <v>1.01353493492812</v>
+      </c>
+      <c r="H13" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I13" s="6">
+        <v>3.37260273972603E-2</v>
+      </c>
+      <c r="J13" s="25">
+        <v>3.2602739726027399</v>
+      </c>
+      <c r="K13" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="24">
+        <v>3.8072685482423099</v>
+      </c>
+      <c r="C14" s="24">
+        <v>5.85589707911471</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1.49952148620754E-2</v>
+      </c>
+      <c r="E14" s="6">
+        <v>3.7280821917808203E-2</v>
+      </c>
+      <c r="F14" s="26">
+        <v>1596.8565966871799</v>
+      </c>
+      <c r="G14" s="24">
+        <v>1.00824731720882</v>
+      </c>
+      <c r="H14" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I14" s="6">
+        <v>3.3849315068493098E-2</v>
+      </c>
+      <c r="J14" s="25">
+        <v>3.3698630136986298</v>
+      </c>
+      <c r="K14" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="24">
+        <v>3.80034763995425</v>
+      </c>
+      <c r="C15" s="24">
+        <v>5.8452521440082599</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1.49952148620754E-2</v>
+      </c>
+      <c r="E15" s="6">
+        <v>3.7342465753424703E-2</v>
+      </c>
+      <c r="F15" s="26">
+        <v>1593.7178262391301</v>
+      </c>
+      <c r="G15" s="24">
+        <v>1.01023302435941</v>
+      </c>
+      <c r="H15" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I15" s="6">
+        <v>3.3910958904109598E-2</v>
+      </c>
+      <c r="J15" s="25">
+        <v>3.3698630136986298</v>
+      </c>
+      <c r="K15" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="24">
+        <v>3.8540419968703699</v>
+      </c>
+      <c r="C16" s="24">
+        <v>6.2216021576406604</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1.4776787389754201E-2</v>
+      </c>
+      <c r="E16" s="6">
+        <v>3.7363013698630099E-2</v>
+      </c>
+      <c r="F16" s="26">
+        <v>1583.3754948936901</v>
+      </c>
+      <c r="G16" s="24">
+        <v>1.0004491193001199</v>
+      </c>
+      <c r="H16" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I16" s="6">
+        <v>3.3849315068493098E-2</v>
+      </c>
+      <c r="J16" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K16" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="24">
+        <v>3.8470360631253002</v>
+      </c>
+      <c r="C17" s="24">
+        <v>6.2102924385094198</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1.4776787389754201E-2</v>
+      </c>
+      <c r="E17" s="6">
+        <v>3.7424657534246598E-2</v>
+      </c>
+      <c r="F17" s="26">
+        <v>1580.2571623809399</v>
+      </c>
+      <c r="G17" s="24">
+        <v>1.0024233125455799</v>
+      </c>
+      <c r="H17" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I17" s="6">
+        <v>3.3910958904109598E-2</v>
+      </c>
+      <c r="J17" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K17" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="24">
+        <v>3.8400555541397901</v>
+      </c>
+      <c r="C18" s="24">
+        <v>6.1990237627137397</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1.4776787389754201E-2</v>
+      </c>
+      <c r="E18" s="6">
+        <v>3.7486301369863001E-2</v>
+      </c>
+      <c r="F18" s="26">
+        <v>1577.1510875301199</v>
+      </c>
+      <c r="G18" s="24">
+        <v>1.004397506309</v>
+      </c>
+      <c r="H18" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I18" s="6">
+        <v>3.3972602739726E-2</v>
+      </c>
+      <c r="J18" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K18" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="24">
+        <v>3.8331003317636001</v>
+      </c>
+      <c r="C19" s="24">
+        <v>6.1877959072369002</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1.4776787389754201E-2</v>
+      </c>
+      <c r="E19" s="6">
+        <v>3.7547945205479501E-2</v>
+      </c>
+      <c r="F19" s="26">
+        <v>1574.0571982003</v>
+      </c>
+      <c r="G19" s="24">
+        <v>1.00637170059573</v>
+      </c>
+      <c r="H19" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I19" s="6">
+        <v>3.40342465753425E-2</v>
+      </c>
+      <c r="J19" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K19" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="24">
+        <v>3.83527602070484</v>
+      </c>
+      <c r="C20" s="24">
+        <v>5.89897491145266</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1.4807187089510201E-2</v>
+      </c>
+      <c r="E20" s="6">
+        <v>3.7589041095890403E-2</v>
+      </c>
+      <c r="F20" s="26">
+        <v>1607.4221082751999</v>
+      </c>
+      <c r="G20" s="24">
+        <v>1.00162015396482</v>
+      </c>
+      <c r="H20" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I20" s="6">
+        <v>3.4157534246575298E-2</v>
+      </c>
+      <c r="J20" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K20" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="24">
+        <v>3.8261702588455901</v>
+      </c>
+      <c r="C21" s="24">
+        <v>6.176608650675</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1.4776787389754201E-2</v>
+      </c>
+      <c r="E21" s="6">
+        <v>3.7609589041095903E-2</v>
+      </c>
+      <c r="F21" s="26">
+        <v>1570.9754228156701</v>
+      </c>
+      <c r="G21" s="24">
+        <v>1.00834589541102</v>
+      </c>
+      <c r="H21" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I21" s="6">
+        <v>3.4095890410958903E-2</v>
+      </c>
+      <c r="J21" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K21" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="24">
+        <v>3.82836699664833</v>
+      </c>
+      <c r="C22" s="24">
+        <v>5.8883482552871103</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1.4807187089510201E-2</v>
+      </c>
+      <c r="E22" s="6">
+        <v>3.7650684931506903E-2</v>
+      </c>
+      <c r="F22" s="26">
+        <v>1604.29331520043</v>
+      </c>
+      <c r="G22" s="24">
+        <v>1.0035735761798099</v>
+      </c>
+      <c r="H22" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I22" s="6">
+        <v>3.4219178082191798E-2</v>
+      </c>
+      <c r="J22" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K22" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="24">
+        <v>3.8192651992246498</v>
+      </c>
+      <c r="C23" s="24">
+        <v>6.1654617732224102</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1.4776787389754201E-2</v>
+      </c>
+      <c r="E23" s="6">
+        <v>3.7671232876712299E-2</v>
+      </c>
+      <c r="F23" s="26">
+        <v>1567.9056903600499</v>
+      </c>
+      <c r="G23" s="24">
+        <v>1.01032009076006</v>
+      </c>
+      <c r="H23" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I23" s="6">
+        <v>3.4157534246575298E-2</v>
+      </c>
+      <c r="J23" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K23" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="24">
+        <v>3.9397850470779501</v>
+      </c>
+      <c r="C24" s="24">
+        <v>6.3600176566433699</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1.4892006004878999E-2</v>
+      </c>
+      <c r="E24" s="6">
+        <v>3.7698630136986301E-2</v>
+      </c>
+      <c r="F24" s="26">
+        <v>1581.1512608850701</v>
+      </c>
+      <c r="G24" s="24">
+        <v>1.00130638837852</v>
+      </c>
+      <c r="H24" s="23">
+        <v>3.54109589041096E-3</v>
+      </c>
+      <c r="I24" s="6">
+        <v>3.4157534246575298E-2</v>
+      </c>
+      <c r="J24" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K24" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="24">
+        <v>3.8214828202307798</v>
+      </c>
+      <c r="C25" s="24">
+        <v>5.8777598168660097</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1.4807187089510201E-2</v>
+      </c>
+      <c r="E25" s="6">
+        <v>3.7712328767123299E-2</v>
+      </c>
+      <c r="F25" s="26">
+        <v>1601.1766776740601</v>
+      </c>
+      <c r="G25" s="24">
+        <v>1.00552699900417</v>
+      </c>
+      <c r="H25" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I25" s="6">
+        <v>3.42808219178082E-2</v>
+      </c>
+      <c r="J25" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K25" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="24">
+        <v>3.81238501772085</v>
+      </c>
+      <c r="C26" s="24">
+        <v>6.1543550566573604</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1.4776787389754201E-2</v>
+      </c>
+      <c r="E26" s="6">
+        <v>3.7732876712328799E-2</v>
+      </c>
+      <c r="F26" s="26">
+        <v>1564.84793037144</v>
+      </c>
+      <c r="G26" s="24">
+        <v>1.0122942866478899</v>
+      </c>
+      <c r="H26" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I26" s="6">
+        <v>3.4219178082191798E-2</v>
+      </c>
+      <c r="J26" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K26" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="24">
+        <v>3.9326877561604801</v>
+      </c>
+      <c r="C27" s="24">
+        <v>6.3485604591033802</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1.4892006004878999E-2</v>
+      </c>
+      <c r="E27" s="6">
+        <v>3.7760273972602697E-2</v>
+      </c>
+      <c r="F27" s="26">
+        <v>1578.06568569465</v>
+      </c>
+      <c r="G27" s="24">
+        <v>1.0032642321983301</v>
+      </c>
+      <c r="H27" s="23">
+        <v>3.54109589041096E-3</v>
+      </c>
+      <c r="I27" s="6">
+        <v>3.4219178082191798E-2</v>
+      </c>
+      <c r="J27" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K27" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="24">
+        <v>3.81462335764959</v>
+      </c>
+      <c r="C28" s="24">
+        <v>5.8672093903897897</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1.4807187089510201E-2</v>
+      </c>
+      <c r="E28" s="6">
+        <v>3.7773972602739701E-2</v>
+      </c>
+      <c r="F28" s="26">
+        <v>1598.0721249897101</v>
+      </c>
+      <c r="G28" s="24">
+        <v>1.0074804224417799</v>
+      </c>
+      <c r="H28" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I28" s="6">
+        <v>3.43424657534247E-2</v>
+      </c>
+      <c r="J28" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K28" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="24">
+        <v>3.8055295801265401</v>
+      </c>
+      <c r="C29" s="24">
+        <v>6.1432882843277001</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1.4776787389754201E-2</v>
+      </c>
+      <c r="E29" s="6">
+        <v>3.7794520547945201E-2</v>
+      </c>
+      <c r="F29" s="26">
+        <v>1561.8020729365799</v>
+      </c>
+      <c r="G29" s="24">
+        <v>1.0142684830794899</v>
+      </c>
+      <c r="H29" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I29" s="6">
+        <v>3.42808219178082E-2</v>
+      </c>
+      <c r="J29" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K29" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="24">
+        <v>3.9256159899655798</v>
+      </c>
+      <c r="C30" s="24">
+        <v>6.3371444662698302</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1.4892006004878999E-2</v>
+      </c>
+      <c r="E30" s="6">
+        <v>3.7821917808219203E-2</v>
+      </c>
+      <c r="F30" s="26">
+        <v>1574.9921290823099</v>
+      </c>
+      <c r="G30" s="24">
+        <v>1.00522207653155</v>
+      </c>
+      <c r="H30" s="23">
+        <v>3.54109589041096E-3</v>
+      </c>
+      <c r="I30" s="6">
+        <v>3.42808219178082E-2</v>
+      </c>
+      <c r="J30" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K30" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="24">
+        <v>3.80778847606113</v>
+      </c>
+      <c r="C31" s="24">
+        <v>5.8566967715338301</v>
+      </c>
+      <c r="D31" s="6">
+        <v>1.4807187089510201E-2</v>
+      </c>
+      <c r="E31" s="6">
+        <v>3.7835616438356201E-2</v>
+      </c>
+      <c r="F31" s="26">
+        <v>1594.9795869884301</v>
+      </c>
+      <c r="G31" s="24">
+        <v>1.0094338464964501</v>
+      </c>
+      <c r="H31" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I31" s="6">
+        <v>3.4404109589041103E-2</v>
+      </c>
+      <c r="J31" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K31" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="24">
+        <v>3.9308586219878001</v>
+      </c>
+      <c r="C32" s="24">
+        <v>6.0459889370131803</v>
+      </c>
+      <c r="D32" s="6">
+        <v>1.49254081441171E-2</v>
+      </c>
+      <c r="E32" s="6">
+        <v>3.7863013698630099E-2</v>
+      </c>
+      <c r="F32" s="26">
+        <v>1608.74198499463</v>
+      </c>
+      <c r="G32" s="24">
+        <v>1.00021719977891</v>
+      </c>
+      <c r="H32" s="23">
+        <v>3.4589041095890402E-3</v>
+      </c>
+      <c r="I32" s="6">
+        <v>3.4404109589041103E-2</v>
+      </c>
+      <c r="J32" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K32" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="24">
+        <v>3.91856961104462</v>
+      </c>
+      <c r="C33" s="24">
+        <v>6.3257694562585698</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1.4892006004878999E-2</v>
+      </c>
+      <c r="E33" s="6">
+        <v>3.7883561643835599E-2</v>
+      </c>
+      <c r="F33" s="26">
+        <v>1571.9305209564</v>
+      </c>
+      <c r="G33" s="24">
+        <v>1.0071799213833601</v>
+      </c>
+      <c r="H33" s="23">
+        <v>3.54109589041096E-3</v>
+      </c>
+      <c r="I33" s="6">
+        <v>3.43424657534247E-2</v>
+      </c>
+      <c r="J33" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K33" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="24">
+        <v>3.8009780435721501</v>
+      </c>
+      <c r="C34" s="24">
+        <v>5.8462217574353001</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1.4807187089510201E-2</v>
+      </c>
+      <c r="E34" s="6">
+        <v>3.7897260273972597E-2</v>
+      </c>
+      <c r="F34" s="26">
+        <v>1591.89899405345</v>
+      </c>
+      <c r="G34" s="24">
+        <v>1.0113872711719301</v>
+      </c>
+      <c r="H34" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I34" s="6">
+        <v>3.4465753424657498E-2</v>
+      </c>
+      <c r="J34" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K34" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="24">
+        <v>3.8578383595086998</v>
+      </c>
+      <c r="C35" s="24">
+        <v>6.2277306476781398</v>
+      </c>
+      <c r="D35" s="6">
+        <v>1.45842559579658E-2</v>
+      </c>
+      <c r="E35" s="6">
+        <v>3.7917808219178097E-2</v>
+      </c>
+      <c r="F35" s="26">
+        <v>1582.8022372876501</v>
+      </c>
+      <c r="G35" s="24">
+        <v>1.0008114608823999</v>
+      </c>
+      <c r="H35" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I35" s="6">
+        <v>3.4404109589041103E-2</v>
+      </c>
+      <c r="J35" s="25">
+        <v>3.1506849315068499</v>
+      </c>
+      <c r="K35" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="24">
+        <v>3.9238280719882201</v>
+      </c>
+      <c r="C36" s="24">
+        <v>6.0351753637951502</v>
+      </c>
+      <c r="D36" s="6">
+        <v>1.49254081441171E-2</v>
+      </c>
+      <c r="E36" s="6">
+        <v>3.7924657534246599E-2</v>
+      </c>
+      <c r="F36" s="26">
+        <v>1605.6328322572401</v>
+      </c>
+      <c r="G36" s="24">
+        <v>1.0021540236792501</v>
+      </c>
+      <c r="H36" s="23">
+        <v>3.4589041095890402E-3</v>
+      </c>
+      <c r="I36" s="6">
+        <v>3.4465753424657498E-2</v>
+      </c>
+      <c r="J36" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K36" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="24">
+        <v>3.9115484829340499</v>
+      </c>
+      <c r="C37" s="24">
+        <v>6.3144352087757296</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1.4892006004878999E-2</v>
+      </c>
+      <c r="E37" s="6">
+        <v>3.7945205479452099E-2</v>
+      </c>
+      <c r="F37" s="26">
+        <v>1568.88079176939</v>
+      </c>
+      <c r="G37" s="24">
+        <v>1.0091377667588199</v>
+      </c>
+      <c r="H37" s="23">
+        <v>3.54109589041096E-3</v>
+      </c>
+      <c r="I37" s="6">
+        <v>3.4404109589041103E-2</v>
+      </c>
+      <c r="J37" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K37" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="24">
+        <v>3.8641451834955398</v>
+      </c>
+      <c r="C38" s="24">
+        <v>5.7138671401851999</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1.49407956464628E-2</v>
+      </c>
+      <c r="E38" s="6">
+        <v>3.7965753424657502E-2</v>
+      </c>
+      <c r="F38" s="26">
+        <v>1630.30033093867</v>
+      </c>
+      <c r="G38" s="24">
+        <v>1.0012600843628501</v>
+      </c>
+      <c r="H38" s="23">
+        <v>3.3767123287671199E-3</v>
+      </c>
+      <c r="I38" s="6">
+        <v>3.4589041095890401E-2</v>
+      </c>
+      <c r="J38" s="25">
+        <v>3.4246575342465801</v>
+      </c>
+      <c r="K38" s="25">
+        <v>62.671232876712303</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="24">
+        <v>3.8509384101375601</v>
+      </c>
+      <c r="C39" s="24">
+        <v>6.2165920197311797</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1.45842559579658E-2</v>
+      </c>
+      <c r="E39" s="6">
+        <v>3.7979452054794499E-2</v>
+      </c>
+      <c r="F39" s="26">
+        <v>1579.7393158104801</v>
+      </c>
+      <c r="G39" s="24">
+        <v>1.00275191199826</v>
+      </c>
+      <c r="H39" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I39" s="6">
+        <v>3.4465753424657498E-2</v>
+      </c>
+      <c r="J39" s="25">
+        <v>3.1506849315068499</v>
+      </c>
+      <c r="K39" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="24">
+        <v>3.9168226261147998</v>
+      </c>
+      <c r="C40" s="24">
+        <v>6.0244004028203104</v>
+      </c>
+      <c r="D40" s="6">
+        <v>1.49254081441171E-2</v>
+      </c>
+      <c r="E40" s="6">
+        <v>3.7986301369863001E-2</v>
+      </c>
+      <c r="F40" s="26">
+        <v>1602.5356732600601</v>
+      </c>
+      <c r="G40" s="24">
+        <v>1.0040908481773201</v>
+      </c>
+      <c r="H40" s="23">
+        <v>3.4589041095890402E-3</v>
+      </c>
+      <c r="I40" s="6">
+        <v>3.4527397260273998E-2</v>
+      </c>
+      <c r="J40" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K40" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="24">
+        <v>3.9045524701466099</v>
+      </c>
+      <c r="C41" s="24">
+        <v>6.3031415051034401</v>
+      </c>
+      <c r="D41" s="6">
+        <v>1.4892006004878999E-2</v>
+      </c>
+      <c r="E41" s="6">
+        <v>3.8006849315068501E-2</v>
+      </c>
+      <c r="F41" s="26">
+        <v>1565.8428725126</v>
+      </c>
+      <c r="G41" s="24">
+        <v>1.0110956126629</v>
+      </c>
+      <c r="H41" s="23">
+        <v>3.54109589041096E-3</v>
+      </c>
+      <c r="I41" s="6">
+        <v>3.4465753424657498E-2</v>
+      </c>
+      <c r="J41" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K41" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="24">
+        <v>3.8572708394252699</v>
+      </c>
+      <c r="C42" s="24">
+        <v>5.7037021264944201</v>
+      </c>
+      <c r="D42" s="6">
+        <v>1.49407956464628E-2</v>
+      </c>
+      <c r="E42" s="6">
+        <v>3.8027397260274001E-2</v>
+      </c>
+      <c r="F42" s="26">
+        <v>1627.1736115991098</v>
+      </c>
+      <c r="G42" s="24">
+        <v>1.00318407037601</v>
+      </c>
+      <c r="H42" s="23">
+        <v>3.3767123287671199E-3</v>
+      </c>
+      <c r="I42" s="6">
+        <v>3.4650684931506803E-2</v>
+      </c>
+      <c r="J42" s="25">
+        <v>3.4246575342465801</v>
+      </c>
+      <c r="K42" s="25">
+        <v>62.671232876712303</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="24">
+        <v>3.8440630985542898</v>
+      </c>
+      <c r="C43" s="24">
+        <v>6.2054931647068603</v>
+      </c>
+      <c r="D43" s="6">
+        <v>1.45842559579658E-2</v>
+      </c>
+      <c r="E43" s="6">
+        <v>3.8041095890410999E-2</v>
+      </c>
+      <c r="F43" s="26">
+        <v>1576.6882248469701</v>
+      </c>
+      <c r="G43" s="24">
+        <v>1.00469236366723</v>
+      </c>
+      <c r="H43" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I43" s="6">
+        <v>3.4527397260273998E-2</v>
+      </c>
+      <c r="J43" s="25">
+        <v>3.1506849315068499</v>
+      </c>
+      <c r="K43" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="24">
+        <v>3.9098421501474698</v>
+      </c>
+      <c r="C44" s="24">
+        <v>6.0136638476469697</v>
+      </c>
+      <c r="D44" s="6">
+        <v>1.49254081441171E-2</v>
+      </c>
+      <c r="E44" s="6">
+        <v>3.8047945205479397E-2</v>
+      </c>
+      <c r="F44" s="26">
+        <v>1599.45043873074</v>
+      </c>
+      <c r="G44" s="24">
+        <v>1.00602767327696</v>
+      </c>
+      <c r="H44" s="23">
+        <v>3.4589041095890402E-3</v>
+      </c>
+      <c r="I44" s="6">
+        <v>3.4589041095890401E-2</v>
+      </c>
+      <c r="J44" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K44" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="24">
+        <v>3.8975814381626201</v>
+      </c>
+      <c r="C45" s="24">
+        <v>6.2918881280857999</v>
+      </c>
+      <c r="D45" s="6">
+        <v>1.4892006004878999E-2</v>
+      </c>
+      <c r="E45" s="6">
+        <v>3.8068493150684897E-2</v>
+      </c>
+      <c r="F45" s="26">
+        <v>1562.8166947109899</v>
+      </c>
+      <c r="G45" s="24">
+        <v>1.0130534591005</v>
+      </c>
+      <c r="H45" s="23">
+        <v>3.54109589041096E-3</v>
+      </c>
+      <c r="I45" s="6">
+        <v>3.4527397260273998E-2</v>
+      </c>
+      <c r="J45" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K45" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="24">
+        <v>3.8442331801479699</v>
+      </c>
+      <c r="C46" s="24">
+        <v>5.9127517709401198</v>
+      </c>
+      <c r="D46" s="6">
+        <v>1.4619159316944999E-2</v>
+      </c>
+      <c r="E46" s="6">
+        <v>3.8082191780821902E-2</v>
+      </c>
+      <c r="F46" s="26">
+        <v>1609.32867140903</v>
+      </c>
+      <c r="G46" s="24">
+        <v>1.0004335398855599</v>
+      </c>
+      <c r="H46" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I46" s="6">
+        <v>3.4650684931506803E-2</v>
+      </c>
+      <c r="J46" s="25">
+        <v>3.2602739726027399</v>
+      </c>
+      <c r="K46" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="24">
+        <v>3.85042091094168</v>
+      </c>
+      <c r="C47" s="24">
+        <v>5.6935732158514698</v>
+      </c>
+      <c r="D47" s="6">
+        <v>1.49407956464628E-2</v>
+      </c>
+      <c r="E47" s="6">
+        <v>3.8089041095890397E-2</v>
+      </c>
+      <c r="F47" s="26">
+        <v>1624.0588615706101</v>
+      </c>
+      <c r="G47" s="24">
+        <v>1.00510805705269</v>
+      </c>
+      <c r="H47" s="23">
+        <v>3.3767123287671199E-3</v>
+      </c>
+      <c r="I47" s="6">
+        <v>3.4712328767123303E-2</v>
+      </c>
+      <c r="J47" s="25">
+        <v>3.4246575342465801</v>
+      </c>
+      <c r="K47" s="25">
+        <v>62.671232876712303</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="24">
+        <v>3.83721229303212</v>
+      </c>
+      <c r="C48" s="24">
+        <v>6.19443386995788</v>
+      </c>
+      <c r="D48" s="6">
+        <v>1.45842559579658E-2</v>
+      </c>
+      <c r="E48" s="6">
+        <v>3.8102739726027401E-2</v>
+      </c>
+      <c r="F48" s="26">
+        <v>1573.6488959793799</v>
+      </c>
+      <c r="G48" s="24">
+        <v>1.0066328158937301</v>
+      </c>
+      <c r="H48" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I48" s="6">
+        <v>3.4589041095890401E-2</v>
+      </c>
+      <c r="J48" s="25">
+        <v>3.1506849315068499</v>
+      </c>
+      <c r="K48" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="24">
+        <v>3.9028865108212498</v>
+      </c>
+      <c r="C49" s="24">
+        <v>6.0029654933024696</v>
+      </c>
+      <c r="D49" s="6">
+        <v>1.49254081441171E-2</v>
+      </c>
+      <c r="E49" s="6">
+        <v>3.8109589041095897E-2</v>
+      </c>
+      <c r="F49" s="26">
+        <v>1596.3770599295299</v>
+      </c>
+      <c r="G49" s="24">
+        <v>1.0079644989819201</v>
+      </c>
+      <c r="H49" s="23">
+        <v>3.4589041095890402E-3</v>
+      </c>
+      <c r="I49" s="6">
+        <v>3.4650684931506803E-2</v>
+      </c>
+      <c r="J49" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K49" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="24">
+        <v>3.89063525342134</v>
+      </c>
+      <c r="C50" s="24">
+        <v>6.2806748621149504</v>
+      </c>
+      <c r="D50" s="6">
+        <v>1.4892006004878999E-2</v>
+      </c>
+      <c r="E50" s="6">
+        <v>3.8130136986301397E-2</v>
+      </c>
+      <c r="F50" s="26">
+        <v>1559.80219041798</v>
+      </c>
+      <c r="G50" s="24">
+        <v>1.0150113060763899</v>
+      </c>
+      <c r="H50" s="23">
+        <v>3.54109589041096E-3</v>
+      </c>
+      <c r="I50" s="6">
+        <v>3.4589041095890401E-2</v>
+      </c>
+      <c r="J50" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K50" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="24">
+        <v>3.8374064045715399</v>
+      </c>
+      <c r="C51" s="24">
+        <v>5.9022516198078296</v>
+      </c>
+      <c r="D51" s="6">
+        <v>1.4619159316944999E-2</v>
+      </c>
+      <c r="E51" s="6">
+        <v>3.8143835616438401E-2</v>
+      </c>
+      <c r="F51" s="26">
+        <v>1606.2441900701799</v>
+      </c>
+      <c r="G51" s="24">
+        <v>1.00235467902718</v>
+      </c>
+      <c r="H51" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I51" s="6">
+        <v>3.4712328767123303E-2</v>
+      </c>
+      <c r="J51" s="25">
+        <v>3.2602739726027399</v>
+      </c>
+      <c r="K51" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="24">
+        <v>3.8435952682002101</v>
+      </c>
+      <c r="C52" s="24">
+        <v>5.6834802162567</v>
+      </c>
+      <c r="D52" s="6">
+        <v>1.49407956464628E-2</v>
+      </c>
+      <c r="E52" s="6">
+        <v>3.8150684931506897E-2</v>
+      </c>
+      <c r="F52" s="26">
+        <v>1620.9560122508799</v>
+      </c>
+      <c r="G52" s="24">
+        <v>1.00703204439566</v>
+      </c>
+      <c r="H52" s="23">
+        <v>3.3767123287671199E-3</v>
+      </c>
+      <c r="I52" s="6">
+        <v>3.4773972602739699E-2</v>
+      </c>
+      <c r="J52" s="25">
+        <v>3.4246575342465801</v>
+      </c>
+      <c r="K52" s="25">
+        <v>62.671232876712303</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="24">
+        <v>3.8303858627816099</v>
+      </c>
+      <c r="C53" s="24">
+        <v>6.1834139243501198</v>
+      </c>
+      <c r="D53" s="6">
+        <v>1.45842559579658E-2</v>
+      </c>
+      <c r="E53" s="6">
+        <v>3.8164383561643797E-2</v>
+      </c>
+      <c r="F53" s="26">
+        <v>1570.6212613166499</v>
+      </c>
+      <c r="G53" s="24">
+        <v>1.00857326868213</v>
+      </c>
+      <c r="H53" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I53" s="6">
+        <v>3.4650684931506803E-2</v>
+      </c>
+      <c r="J53" s="25">
+        <v>3.1506849315068499</v>
+      </c>
+      <c r="K53" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="24">
+        <v>3.8959555758178199</v>
+      </c>
+      <c r="C54" s="24">
+        <v>5.9923051362701596</v>
+      </c>
+      <c r="D54" s="6">
+        <v>1.49254081441171E-2</v>
+      </c>
+      <c r="E54" s="6">
+        <v>3.8171232876712299E-2</v>
+      </c>
+      <c r="F54" s="26">
+        <v>1593.3154686440998</v>
+      </c>
+      <c r="G54" s="24">
+        <v>1.0099013252958799</v>
+      </c>
+      <c r="H54" s="23">
+        <v>3.4589041095890402E-3</v>
+      </c>
+      <c r="I54" s="6">
+        <v>3.4712328767123303E-2</v>
+      </c>
+      <c r="J54" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K54" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="24">
+        <v>3.88371378331246</v>
+      </c>
+      <c r="C55" s="24">
+        <v>6.2695014931173203</v>
+      </c>
+      <c r="D55" s="6">
+        <v>1.4892006004878999E-2</v>
+      </c>
+      <c r="E55" s="6">
+        <v>3.8191780821917799E-2</v>
+      </c>
+      <c r="F55" s="26">
+        <v>1556.7992922104199</v>
+      </c>
+      <c r="G55" s="24">
+        <v>1.0169691535952901</v>
+      </c>
+      <c r="H55" s="23">
+        <v>3.54109589041096E-3</v>
+      </c>
+      <c r="I55" s="6">
+        <v>3.4650684931506803E-2</v>
+      </c>
+      <c r="J55" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K55" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="24">
+        <v>3.83060383265089</v>
+      </c>
+      <c r="C56" s="24">
+        <v>5.8917886959200496</v>
+      </c>
+      <c r="D56" s="6">
+        <v>1.4619159316944999E-2</v>
+      </c>
+      <c r="E56" s="6">
+        <v>3.8205479452054797E-2</v>
+      </c>
+      <c r="F56" s="26">
+        <v>1603.17150870606</v>
+      </c>
+      <c r="G56" s="24">
+        <v>1.0042758187965399</v>
+      </c>
+      <c r="H56" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I56" s="6">
+        <v>3.4773972602739699E-2</v>
+      </c>
+      <c r="J56" s="25">
+        <v>3.2602739726027399</v>
+      </c>
+      <c r="K56" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="24">
+        <v>3.83679378227535</v>
+      </c>
+      <c r="C57" s="24">
+        <v>5.6734229370694598</v>
+      </c>
+      <c r="D57" s="6">
+        <v>1.49407956464628E-2</v>
+      </c>
+      <c r="E57" s="6">
+        <v>3.8212328767123299E-2</v>
+      </c>
+      <c r="F57" s="26">
+        <v>1617.8649955610399</v>
+      </c>
+      <c r="G57" s="24">
+        <v>1.0089560324076201</v>
+      </c>
+      <c r="H57" s="23">
+        <v>3.3767123287671199E-3</v>
+      </c>
+      <c r="I57" s="6">
+        <v>3.4835616438356198E-2</v>
+      </c>
+      <c r="J57" s="25">
+        <v>3.4246575342465801</v>
+      </c>
+      <c r="K57" s="25">
+        <v>62.671232876712303</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="24">
+        <v>3.8235836779424202</v>
+      </c>
+      <c r="C58" s="24">
+        <v>6.17243311824926</v>
+      </c>
+      <c r="D58" s="6">
+        <v>1.45842559579658E-2</v>
+      </c>
+      <c r="E58" s="6">
+        <v>3.8226027397260297E-2</v>
+      </c>
+      <c r="F58" s="26">
+        <v>1567.6052534893502</v>
+      </c>
+      <c r="G58" s="24">
+        <v>1.01051372203668</v>
+      </c>
+      <c r="H58" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I58" s="6">
+        <v>3.4712328767123303E-2</v>
+      </c>
+      <c r="J58" s="25">
+        <v>3.1506849315068499</v>
+      </c>
+      <c r="K58" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="24">
+        <v>3.8890492137570898</v>
+      </c>
+      <c r="C59" s="24">
+        <v>5.9816825744765003</v>
+      </c>
+      <c r="D59" s="6">
+        <v>1.49254081441171E-2</v>
+      </c>
+      <c r="E59" s="6">
+        <v>3.8232876712328799E-2</v>
+      </c>
+      <c r="F59" s="26">
+        <v>1590.26559718454</v>
+      </c>
+      <c r="G59" s="24">
+        <v>1.01183815222243</v>
+      </c>
+      <c r="H59" s="23">
+        <v>3.4589041095890402E-3</v>
+      </c>
+      <c r="I59" s="6">
+        <v>3.4773972602739699E-2</v>
+      </c>
+      <c r="J59" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K59" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="24">
+        <v>3.9442397987097202</v>
+      </c>
+      <c r="C60" s="24">
+        <v>6.36720898781891</v>
+      </c>
+      <c r="D60" s="6">
+        <v>1.4697973353349599E-2</v>
+      </c>
+      <c r="E60" s="6">
+        <v>3.8253424657534299E-2</v>
+      </c>
+      <c r="F60" s="26">
+        <v>1580.8306798475498</v>
+      </c>
+      <c r="G60" s="24">
+        <v>1.00150944607784</v>
+      </c>
+      <c r="H60" s="23">
+        <v>3.54109589041096E-3</v>
+      </c>
+      <c r="I60" s="6">
+        <v>3.4712328767123303E-2</v>
+      </c>
+      <c r="J60" s="25">
+        <v>3.1506849315068499</v>
+      </c>
+      <c r="K60" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="24">
+        <v>3.8768168961676701</v>
+      </c>
+      <c r="C61" s="24">
+        <v>6.2583678085399601</v>
+      </c>
+      <c r="D61" s="6">
+        <v>1.4892006004878999E-2</v>
+      </c>
+      <c r="E61" s="6">
+        <v>3.8253424657534299E-2</v>
+      </c>
+      <c r="F61" s="26">
+        <v>1553.8079331834901</v>
+      </c>
+      <c r="G61" s="24">
+        <v>1.0189270016617999</v>
+      </c>
+      <c r="H61" s="23">
+        <v>3.54109589041096E-3</v>
+      </c>
+      <c r="I61" s="6">
+        <v>3.4712328767123303E-2</v>
+      </c>
+      <c r="J61" s="25">
+        <v>3.20547945205479</v>
+      </c>
+      <c r="K61" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="24">
+        <v>3.8238253358962999</v>
+      </c>
+      <c r="C62" s="24">
+        <v>5.8813628016488604</v>
+      </c>
+      <c r="D62" s="6">
+        <v>1.4619159316944999E-2</v>
+      </c>
+      <c r="E62" s="6">
+        <v>3.8267123287671199E-2</v>
+      </c>
+      <c r="F62" s="26">
+        <v>1600.11055972794</v>
+      </c>
+      <c r="G62" s="24">
+        <v>1.00619695919688</v>
+      </c>
+      <c r="H62" s="23">
+        <v>3.4315068493150701E-3</v>
+      </c>
+      <c r="I62" s="6">
+        <v>3.4835616438356198E-2</v>
+      </c>
+      <c r="J62" s="25">
+        <v>3.2602739726027399</v>
+      </c>
+      <c r="K62" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="24">
+        <v>3.8300163251525898</v>
+      </c>
+      <c r="C63" s="24">
+        <v>5.6634011889961302</v>
+      </c>
+      <c r="D63" s="6">
+        <v>1.49407956464628E-2</v>
+      </c>
+      <c r="E63" s="6">
+        <v>3.8273972602739702E-2</v>
+      </c>
+      <c r="F63" s="26">
+        <v>1614.7857439405702</v>
+      </c>
+      <c r="G63" s="24">
+        <v>1.0108800210912201</v>
+      </c>
+      <c r="H63" s="23">
+        <v>3.3767123287671199E-3</v>
+      </c>
+      <c r="I63" s="6">
+        <v>3.4897260273972601E-2</v>
+      </c>
+      <c r="J63" s="25">
+        <v>3.4246575342465801</v>
+      </c>
+      <c r="K63" s="25">
+        <v>62.671232876712303</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="24">
+        <v>3.8168056095749798</v>
+      </c>
+      <c r="C64" s="24">
+        <v>6.1614912435074398</v>
+      </c>
+      <c r="D64" s="6">
+        <v>1.45842559579658E-2</v>
+      </c>
+      <c r="E64" s="6">
+        <v>3.8287671232876699E-2</v>
+      </c>
+      <c r="F64" s="26">
+        <v>1564.6008056446499</v>
+      </c>
+      <c r="G64" s="24">
+        <v>1.0124541759615799</v>
+      </c>
+      <c r="H64" s="23">
+        <v>3.5136986301369899E-3</v>
+      </c>
+      <c r="I64" s="6">
+        <v>3.4773972602739699E-2</v>
+      </c>
+      <c r="J64" s="25">
+        <v>3.1506849315068499</v>
+      </c>
+      <c r="K64" s="25">
+        <v>48.835616438356197</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B65" s="24">
+        <v>3.8821672941888998</v>
+      </c>
+      <c r="C65" s="24">
+        <v>5.9710976072782502</v>
+      </c>
+      <c r="D65" s="6">
+        <v>1.49254081441171E-2</v>
+      </c>
+      <c r="E65" s="6">
+        <v>3.8294520547945202E-2</v>
+      </c>
+      <c r="F65" s="26">
+        <v>1587.2273783783301</v>
+      </c>
+      <c r="G65" s="24">
+        <v>1.0137749797650999</v>
+      </c>
+      <c r="H65" s="23">
+        <v>3.4589041095890402E-3</v>
+      </c>
+      <c r="I65" s="6">
+        <v>3.4835616438356198E-2</v>
+      </c>
+      <c r="J65" s="25">
+        <v>3.3150684931506902</v>
+      </c>
+      <c r="K65" s="25">
+        <v>55.753424657534303</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B2:K65">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="14.6E-3"/>
+        <filter val="14.7E-3"/>
+        <filter val="14.8E-3"/>
+        <filter val="14.9E-3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="B3:K65">
+    <sortCondition ref="E3:E65"/>
+    <sortCondition ref="D3:D65"/>
+    <sortCondition descending="1" ref="G3:G65"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added an optional input for adjusting the SOM Matrix size. Trying additional input_data problems (wave spring design).
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -9,18 +9,19 @@
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$B$4:$H$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$B$4:$H$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$B$2:$K$65</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">data!$B$4:$H$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">data!$B$4:$H$18</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -40,15 +41,9 @@
     <t>var</t>
   </si>
   <si>
-    <t>Number of Coils</t>
-  </si>
-  <si>
     <t>con</t>
   </si>
   <si>
-    <t>ad</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -58,279 +53,36 @@
     <t>Nb</t>
   </si>
   <si>
-    <t>ap</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
-    <t>Deflection angle [deg]</t>
-  </si>
-  <si>
-    <t>Prewind Angle [deg]</t>
-  </si>
-  <si>
     <t>Mean Diameter of Coils [m]</t>
   </si>
   <si>
-    <t>Diameter of wire [m]</t>
-  </si>
-  <si>
     <t>M1</t>
   </si>
   <si>
     <t>cst</t>
   </si>
   <si>
-    <t>Moment 1 Constraint [deg]</t>
-  </si>
-  <si>
     <t>M2</t>
   </si>
   <si>
-    <t>Moment 2 Constraint [deg]</t>
-  </si>
-  <si>
     <t>h</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Constant "m" for Sut Eqn (Sut = A/d^m)</t>
-  </si>
-  <si>
-    <t>Youngs Modulus, A877 - VDSiCr, [Pa]</t>
-  </si>
-  <si>
-    <t>db</t>
-  </si>
-  <si>
-    <t>Constant "A" for Sut Eqn (Sut = A/d^m), 2135 Max</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>pi*d^4/64</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Dm/d</t>
-  </si>
-  <si>
     <t>aux</t>
   </si>
   <si>
     <t>k</t>
   </si>
   <si>
-    <t>(pi/180)*(E*I)/(pi*Dm*Nb)</t>
-  </si>
-  <si>
-    <t>k*ap</t>
-  </si>
-  <si>
-    <t>k*(ap+ad)</t>
-  </si>
-  <si>
-    <t>Kb</t>
-  </si>
-  <si>
-    <t>(4*C^2-C-1)/(4*C*(C-1))</t>
-  </si>
-  <si>
-    <t>Spring Pocket Bore [mm]</t>
-  </si>
-  <si>
-    <t>Spring Height [mm]</t>
-  </si>
-  <si>
-    <t>Dm+d</t>
-  </si>
-  <si>
-    <t>obj</t>
-  </si>
-  <si>
-    <t>(Kb*32*M2)/(pi*d^3)</t>
-  </si>
-  <si>
     <t>Sut</t>
   </si>
   <si>
-    <t>A/(d*1e3)^m</t>
-  </si>
-  <si>
-    <t>cs</t>
-  </si>
-  <si>
-    <t>Spring coil spacing [mm]</t>
-  </si>
-  <si>
-    <t>Moment of Inertia, round wire</t>
-  </si>
-  <si>
-    <t>Spring Index</t>
-  </si>
-  <si>
-    <t>Spring Stress Concentration, ID</t>
-  </si>
-  <si>
-    <t>Spring Constant [Nm/deg]</t>
-  </si>
-  <si>
-    <t>Ultimate Strength Calc [Pa]</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
-    <t>Sr</t>
-  </si>
-  <si>
-    <t>0.5*Sut</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>(M2-M1)/2</t>
-  </si>
-  <si>
-    <t>Mm</t>
-  </si>
-  <si>
-    <t>(M2+M1)/2</t>
-  </si>
-  <si>
-    <t>ga</t>
-  </si>
-  <si>
-    <t>gm</t>
-  </si>
-  <si>
-    <t>Sigma_a alternating stress</t>
-  </si>
-  <si>
-    <t>Sigma_m mean stress</t>
-  </si>
-  <si>
-    <t>Alternating Moment</t>
-  </si>
-  <si>
-    <t>Mean Moment</t>
-  </si>
-  <si>
-    <t>gs</t>
-  </si>
-  <si>
-    <t>sigma_s Spring static stress [Pa]</t>
-  </si>
-  <si>
-    <t>(Kb*32*Ma)/(pi*d^3)</t>
-  </si>
-  <si>
-    <t>(Kb*32*Mm)/(pi*d^3)</t>
-  </si>
-  <si>
-    <t>Se</t>
-  </si>
-  <si>
-    <t>Fatigue Strength</t>
-  </si>
-  <si>
-    <t>nf</t>
-  </si>
-  <si>
-    <t>Fatigue factor of safety</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>M1/M2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load Ratio </t>
-  </si>
-  <si>
-    <t>(1+Nb)*(d+cs)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Endurance Strength </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(1) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Sr/2)/(1-((Sr/2)/Sut)^2)</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">From </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mean stress sensitivity of spring steel in the very high cycle fatigue regime - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Schuller 2015</t>
-    </r>
-  </si>
-  <si>
-    <t>nf = (1)*ga/(2*Se)*(Sut/gm)^2*(-1+(1+(2*gm*Se/(Sut*ga))^2)^(0.5))</t>
-  </si>
-  <si>
-    <t>0.9*Sut</t>
-  </si>
-  <si>
     <t>Db</t>
   </si>
   <si>
@@ -343,7 +95,130 @@
     <t>θp</t>
   </si>
   <si>
-    <t>(-1)*(1/((ga/Se)+(gm/Sut)))</t>
+    <t>b</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>OD</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Radial Wall (width) of Material [m]</t>
+  </si>
+  <si>
+    <t>Inside Diameter [m]</t>
+  </si>
+  <si>
+    <t>Multiple Wave Factor</t>
+  </si>
+  <si>
+    <t>Number of Waves per Turn</t>
+  </si>
+  <si>
+    <t>Outside Diameter [m]</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>Static Operating Stress [Pa]</t>
+  </si>
+  <si>
+    <t>Material Thickness [m]</t>
+  </si>
+  <si>
+    <t>Number of Turns</t>
+  </si>
+  <si>
+    <t>Spring Rate [N/m]</t>
+  </si>
+  <si>
+    <t>Kw</t>
+  </si>
+  <si>
+    <t>Dm+b/2</t>
+  </si>
+  <si>
+    <t>Dm-b/2</t>
+  </si>
+  <si>
+    <t>(E*b*t^3*N^4)/(Kw*Dm^3*Z)*(OD/ID)</t>
+  </si>
+  <si>
+    <t>0.0307*N^2-0.648*N+5.5445</t>
+  </si>
+  <si>
+    <t>xo</t>
+  </si>
+  <si>
+    <t>k*(xo)</t>
+  </si>
+  <si>
+    <t>(3*pi*P2*Dm)/(4*b*t^2*N^2)</t>
+  </si>
+  <si>
+    <t>Working Deflection [m]</t>
+  </si>
+  <si>
+    <t>xw</t>
+  </si>
+  <si>
+    <t>k*(xo+xw)</t>
+  </si>
+  <si>
+    <t>Ball Diameter [m]</t>
+  </si>
+  <si>
+    <t>Pressure at position 1 [Pa]</t>
+  </si>
+  <si>
+    <t>Pressure at position 2 [Pa]</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>Force at position 1 [N]</t>
+  </si>
+  <si>
+    <t>Force at position 2 [N]</t>
+  </si>
+  <si>
+    <t>F1/(pi*Db^2/2)</t>
+  </si>
+  <si>
+    <t>F2/(pi*Db^2/2)</t>
+  </si>
+  <si>
+    <t>Pre-Load Deflection [m]</t>
+  </si>
+  <si>
+    <t>Youngs Modulus,17-7 SS [Pa]</t>
+  </si>
+  <si>
+    <t>Tensile Strength [Pa]</t>
   </si>
 </sst>
 </file>
@@ -351,11 +226,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="##0.000E+0"/>
     <numFmt numFmtId="165" formatCode="##0.00E+0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="##0E+0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,22 +240,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -430,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -446,27 +305,10 @@
     <xf numFmtId="48" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="48" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -487,8 +329,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,6 +353,190 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:forward val="1"/>
+            <c:backward val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5585083114610672E-2"/>
+                  <c:y val="6.6505905511811028E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$6:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$6:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="110808448"/>
+        <c:axId val="110806912"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="110808448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="110806912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="110806912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="110808448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -794,10 +829,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B4:L31"/>
+  <dimension ref="B4:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,22 +840,22 @@
     <col min="1" max="1" width="2.140625" customWidth="1"/>
     <col min="2" max="2" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.42578125" customWidth="1"/>
     <col min="11" max="11" width="2.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>1</v>
@@ -834,632 +869,474 @@
       <c r="H4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="K4" s="14">
+      <c r="I4" s="9"/>
+      <c r="K4" s="8">
         <v>1</v>
       </c>
-      <c r="L4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6">
-        <v>3.6218605889890582E-3</v>
+        <v>5.1000000000000004E-4</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="G5" s="7">
-        <v>4.4999999999999997E-3</v>
+      <c r="F5" s="23">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="G5" s="22">
+        <v>2E-3</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="17"/>
+        <v>32</v>
+      </c>
+      <c r="I5" s="10"/>
       <c r="K5">
         <v>2</v>
       </c>
-      <c r="L5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="6">
-        <v>3.4678117394444263E-2</v>
+        <v>4.5100000000000001E-3</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="7">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="G6" s="7">
-        <v>3.6499999999999998E-2</v>
+      <c r="F6" s="22">
+        <v>3.2499999999999999E-3</v>
+      </c>
+      <c r="G6" s="22">
+        <v>5.7499999999999999E-3</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="17"/>
+        <v>11</v>
+      </c>
+      <c r="I6" s="10"/>
       <c r="K6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="8">
-        <v>3.1415154578360882</v>
+        <v>28</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2.5</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="17"/>
+        <v>35</v>
+      </c>
+      <c r="I7" s="10"/>
       <c r="K7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="8">
-        <v>42.823990013566025</v>
+        <v>30</v>
+      </c>
+      <c r="D8" s="24">
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="2">
-        <v>35</v>
-      </c>
-      <c r="G8" s="2">
-        <v>540</v>
+      <c r="F8" s="23">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="G8" s="23">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="9">
-        <v>2204156000</v>
+        <v>31</v>
+      </c>
+      <c r="D9" s="7">
+        <v>3</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>10</v>
+      </c>
       <c r="H9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="17"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.10630000000000001</v>
+        <v>48</v>
+      </c>
+      <c r="D10" s="6">
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="F10" s="23">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G10" s="22">
+        <v>0.01</v>
+      </c>
       <c r="H10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="17"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>7</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="6">
-        <v>206000000000</v>
+        <v>52</v>
+      </c>
+      <c r="D11" s="16">
+        <v>2E-3</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="17"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>8</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="8">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="D12" s="16">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="17"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>9</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="D13" s="16">
+        <v>203400000000</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I13" s="17"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>31</v>
+        <v>18</v>
+      </c>
+      <c r="D14" s="16">
+        <v>1650000000</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="20">
-        <f>PI()*D5^4/64</f>
-        <v>8.4468895846728925E-12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>11</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="22">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G15" s="22"/>
+      <c r="H15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="17"/>
-      <c r="J15" s="20">
-        <f>D6/D5</f>
-        <v>9.574669301151566</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I15" s="10"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>12</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>40</v>
+        <v>26</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22">
+        <v>6.0000000000000001E-3</v>
+      </c>
       <c r="H16" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="20">
-        <f>(4*J15^2-J15-1)/(4*J15*(J15-1))</f>
-        <v>1.0844218490768605</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="13"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>13</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="20">
-        <f>(PI()/180)*(D11*J14)/(PI()*D6*D7)</f>
-        <v>8.8735381139592465E-2</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="13"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>14</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>37</v>
+        <v>17</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="2">
-        <v>3.8</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="17"/>
-      <c r="J18" s="21">
-        <f>J17*D8</f>
-        <v>3.8000030757718828</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="13"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>15</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>38</v>
+        <v>57</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2">
-        <v>6.5</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="17"/>
-      <c r="J19" s="21">
-        <f>J17*(D8+D12)</f>
-        <v>6.4620645099596574</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="14"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>79</v>
+        <v>58</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="7">
-        <v>1.4999999999999999E-2</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
       <c r="H20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="20">
-        <f>(1+D7)*(D5+D13)</f>
-        <v>1.4999991615425503E-2</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="14"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <v>17</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="7">
-        <v>3.8300000000000001E-2</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F21" s="22">
+        <v>60000</v>
+      </c>
+      <c r="G21" s="22"/>
       <c r="H21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="20">
-        <f>D6+D5</f>
-        <v>3.829997798343332E-2</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="I21" s="10"/>
+      <c r="J21" s="13"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <v>18</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>47</v>
+        <v>38</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I22" s="18"/>
+        <v>16</v>
+      </c>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22">
+        <v>120000</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="10"/>
+      <c r="J22" s="13"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>19</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>45</v>
+        <v>29</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F23" s="2"/>
-      <c r="G23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="22">
-        <f>(J16*32*J19)/(PI()*D5^3)/1000000</f>
-        <v>1502.3615673139459</v>
-      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="11"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="4">
-        <v>20</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="I24" s="19"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="15"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
-        <v>21</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I25" s="19"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
-        <v>22</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I26" s="19"/>
+      <c r="I26" s="12"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="4">
-        <v>23</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I27" s="17"/>
+      <c r="I27" s="12"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="4">
-        <v>24</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I28" s="17"/>
-    </row>
-    <row r="29" spans="2:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="4">
-        <v>25</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="15">
-        <v>900000000</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I29" s="17"/>
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I29" s="10"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="4">
-        <v>26</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="5">
-        <v>1</v>
-      </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I30" s="17"/>
+      <c r="I30" s="10"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="4">
-        <v>27</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="I31" s="19"/>
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I32" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:H31"/>
+  <autoFilter ref="B4:H18">
+    <sortState ref="B5:H17">
+      <sortCondition descending="1" ref="E4:E17"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1488,42 +1365,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="27" t="s">
+      <c r="B2" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="G2" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="3" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24">
+      <c r="B3" s="17">
         <v>3.84529021651753</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="17">
         <v>6.2074741082912697</v>
       </c>
       <c r="D3" s="6">
@@ -1532,30 +1409,30 @@
       <c r="E3" s="6">
         <v>3.6869863013698601E-2</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="19">
         <v>1581.7340891706499</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="17">
         <v>1.00148731081491</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I3" s="6">
         <v>3.33561643835616E-2</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="18">
         <v>3.2602739726027399</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="4" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="24">
+      <c r="B4" s="17">
         <v>3.8381970392376199</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="17">
         <v>6.1960235514200601</v>
       </c>
       <c r="D4" s="6">
@@ -1564,30 +1441,30 @@
       <c r="E4" s="6">
         <v>3.69315068493151E-2</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="19">
         <v>1578.5691304524701</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="17">
         <v>1.0034952469479299</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I4" s="6">
         <v>3.34178082191781E-2</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="18">
         <v>3.2602739726027399</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="5" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="24">
+      <c r="B5" s="17">
         <v>3.8311299824959799</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="17">
         <v>6.1846151610839701</v>
       </c>
       <c r="D5" s="6">
@@ -1596,30 +1473,30 @@
       <c r="E5" s="6">
         <v>3.6993150684931503E-2</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="19">
         <v>1575.4168114901499</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="17">
         <v>1.0055031835603101</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I5" s="6">
         <v>3.3479452054794502E-2</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="18">
         <v>3.2602739726027399</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="6" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="24">
+      <c r="B6" s="17">
         <v>3.8352061079114401</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="17">
         <v>5.8988673797360196</v>
       </c>
       <c r="D6" s="6">
@@ -1628,30 +1505,30 @@
       <c r="E6" s="6">
         <v>3.7034246575342503E-2</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="19">
         <v>1609.53628463168</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="17">
         <v>1.0003044944994799</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I6" s="6">
         <v>3.3602739726027397E-2</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="18">
         <v>3.3698630136986298</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="7" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="24">
+      <c r="B7" s="17">
         <v>3.82408890227493</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="17">
         <v>6.1732487047944602</v>
       </c>
       <c r="D7" s="6">
@@ -1660,30 +1537,30 @@
       <c r="E7" s="6">
         <v>3.7054794520548003E-2</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="19">
         <v>1572.2770567064699</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="17">
         <v>1.00751112065837</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I7" s="6">
         <v>3.3541095890411002E-2</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="18">
         <v>3.2602739726027399</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="8" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="24">
+      <c r="B8" s="17">
         <v>3.82818335003327</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="17">
         <v>5.8880657914516599</v>
       </c>
       <c r="D8" s="6">
@@ -1692,30 +1569,30 @@
       <c r="E8" s="6">
         <v>3.7095890410958898E-2</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="19">
         <v>1606.3475235994599</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="17">
         <v>1.00229019930218</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I8" s="6">
         <v>3.36643835616438E-2</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="18">
         <v>3.3698630136986298</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="9" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="24">
+      <c r="B9" s="17">
         <v>3.8170736556136098</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="17">
         <v>6.1619239517689497</v>
       </c>
       <c r="D9" s="6">
@@ -1724,30 +1601,30 @@
       <c r="E9" s="6">
         <v>3.7116438356164398E-2</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="19">
         <v>1569.14979112572</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="17">
         <v>1.00951905824832</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I9" s="6">
         <v>3.3602739726027397E-2</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="18">
         <v>3.2602739726027399</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="10" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="24">
+      <c r="B10" s="17">
         <v>3.82118626430006</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="17">
         <v>5.8773036890708603</v>
       </c>
       <c r="D10" s="6">
@@ -1756,30 +1633,30 @@
       <c r="E10" s="6">
         <v>3.7157534246575301E-2</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="19">
         <v>1603.17137159868</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="17">
         <v>1.00427590468482</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I10" s="6">
         <v>3.37260273972603E-2</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="18">
         <v>3.3698630136986298</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="11" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="24">
+      <c r="B11" s="17">
         <v>3.8100841005982402</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="17">
         <v>6.1506406729152499</v>
       </c>
       <c r="D11" s="6">
@@ -1788,30 +1665,30 @@
       <c r="E11" s="6">
         <v>3.7178082191780801E-2</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="19">
         <v>1566.0349403677399</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="17">
         <v>1.0115269963362401</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I11" s="6">
         <v>3.36643835616438E-2</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="18">
         <v>3.2602739726027399</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K11" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="12" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="24">
+      <c r="B12" s="17">
         <v>3.8142147101993702</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="17">
         <v>5.8665808564737301</v>
       </c>
       <c r="D12" s="6">
@@ -1820,30 +1697,30 @@
       <c r="E12" s="6">
         <v>3.7219178082191801E-2</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="19">
         <v>1600.00775398121</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="17">
         <v>1.00626161065215</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I12" s="6">
         <v>3.3787671232876702E-2</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="18">
         <v>3.3698630136986298</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="13" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="24">
+      <c r="B13" s="17">
         <v>3.8031200963526302</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="17">
         <v>6.1393986408160997</v>
       </c>
       <c r="D13" s="6">
@@ -1852,30 +1729,30 @@
       <c r="E13" s="6">
         <v>3.72397260273973E-2</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="19">
         <v>1562.9324306419899</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="17">
         <v>1.01353493492812</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I13" s="6">
         <v>3.37260273972603E-2</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13" s="18">
         <v>3.2602739726027399</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="14" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="24">
+      <c r="B14" s="17">
         <v>3.8072685482423099</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="17">
         <v>5.85589707911471</v>
       </c>
       <c r="D14" s="6">
@@ -1884,30 +1761,30 @@
       <c r="E14" s="6">
         <v>3.7280821917808203E-2</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="19">
         <v>1596.8565966871799</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="17">
         <v>1.00824731720882</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I14" s="6">
         <v>3.3849315068493098E-2</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="18">
         <v>3.3698630136986298</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="15" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="24">
+      <c r="B15" s="17">
         <v>3.80034763995425</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="17">
         <v>5.8452521440082599</v>
       </c>
       <c r="D15" s="6">
@@ -1916,30 +1793,30 @@
       <c r="E15" s="6">
         <v>3.7342465753424703E-2</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="19">
         <v>1593.7178262391301</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="17">
         <v>1.01023302435941</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I15" s="6">
         <v>3.3910958904109598E-2</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15" s="18">
         <v>3.3698630136986298</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="24">
+      <c r="B16" s="17">
         <v>3.8540419968703699</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="17">
         <v>6.2216021576406604</v>
       </c>
       <c r="D16" s="6">
@@ -1948,30 +1825,30 @@
       <c r="E16" s="6">
         <v>3.7363013698630099E-2</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="19">
         <v>1583.3754948936901</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="17">
         <v>1.0004491193001199</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I16" s="6">
         <v>3.3849315068493098E-2</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J16" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="24">
+      <c r="B17" s="17">
         <v>3.8470360631253002</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="17">
         <v>6.2102924385094198</v>
       </c>
       <c r="D17" s="6">
@@ -1980,30 +1857,30 @@
       <c r="E17" s="6">
         <v>3.7424657534246598E-2</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="19">
         <v>1580.2571623809399</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="17">
         <v>1.0024233125455799</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I17" s="6">
         <v>3.3910958904109598E-2</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="24">
+      <c r="B18" s="17">
         <v>3.8400555541397901</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="17">
         <v>6.1990237627137397</v>
       </c>
       <c r="D18" s="6">
@@ -2012,30 +1889,30 @@
       <c r="E18" s="6">
         <v>3.7486301369863001E-2</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="19">
         <v>1577.1510875301199</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="17">
         <v>1.004397506309</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I18" s="6">
         <v>3.3972602739726E-2</v>
       </c>
-      <c r="J18" s="25">
+      <c r="J18" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="24">
+      <c r="B19" s="17">
         <v>3.8331003317636001</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="17">
         <v>6.1877959072369002</v>
       </c>
       <c r="D19" s="6">
@@ -2044,30 +1921,30 @@
       <c r="E19" s="6">
         <v>3.7547945205479501E-2</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="19">
         <v>1574.0571982003</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="17">
         <v>1.00637170059573</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I19" s="6">
         <v>3.40342465753425E-2</v>
       </c>
-      <c r="J19" s="25">
+      <c r="J19" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="24">
+      <c r="B20" s="17">
         <v>3.83527602070484</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C20" s="17">
         <v>5.89897491145266</v>
       </c>
       <c r="D20" s="6">
@@ -2076,30 +1953,30 @@
       <c r="E20" s="6">
         <v>3.7589041095890403E-2</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="19">
         <v>1607.4221082751999</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="17">
         <v>1.00162015396482</v>
       </c>
-      <c r="H20" s="23">
+      <c r="H20" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I20" s="6">
         <v>3.4157534246575298E-2</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="24">
+      <c r="B21" s="17">
         <v>3.8261702588455901</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="17">
         <v>6.176608650675</v>
       </c>
       <c r="D21" s="6">
@@ -2108,30 +1985,30 @@
       <c r="E21" s="6">
         <v>3.7609589041095903E-2</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="19">
         <v>1570.9754228156701</v>
       </c>
-      <c r="G21" s="24">
+      <c r="G21" s="17">
         <v>1.00834589541102</v>
       </c>
-      <c r="H21" s="23">
+      <c r="H21" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I21" s="6">
         <v>3.4095890410958903E-2</v>
       </c>
-      <c r="J21" s="25">
+      <c r="J21" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K21" s="25">
+      <c r="K21" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="24">
+      <c r="B22" s="17">
         <v>3.82836699664833</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="17">
         <v>5.8883482552871103</v>
       </c>
       <c r="D22" s="6">
@@ -2140,30 +2017,30 @@
       <c r="E22" s="6">
         <v>3.7650684931506903E-2</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="19">
         <v>1604.29331520043</v>
       </c>
-      <c r="G22" s="24">
+      <c r="G22" s="17">
         <v>1.0035735761798099</v>
       </c>
-      <c r="H22" s="23">
+      <c r="H22" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I22" s="6">
         <v>3.4219178082191798E-2</v>
       </c>
-      <c r="J22" s="25">
+      <c r="J22" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K22" s="25">
+      <c r="K22" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="24">
+      <c r="B23" s="17">
         <v>3.8192651992246498</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="17">
         <v>6.1654617732224102</v>
       </c>
       <c r="D23" s="6">
@@ -2172,30 +2049,30 @@
       <c r="E23" s="6">
         <v>3.7671232876712299E-2</v>
       </c>
-      <c r="F23" s="26">
+      <c r="F23" s="19">
         <v>1567.9056903600499</v>
       </c>
-      <c r="G23" s="24">
+      <c r="G23" s="17">
         <v>1.01032009076006</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H23" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I23" s="6">
         <v>3.4157534246575298E-2</v>
       </c>
-      <c r="J23" s="25">
+      <c r="J23" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="24">
+      <c r="B24" s="17">
         <v>3.9397850470779501</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="17">
         <v>6.3600176566433699</v>
       </c>
       <c r="D24" s="6">
@@ -2204,30 +2081,30 @@
       <c r="E24" s="6">
         <v>3.7698630136986301E-2</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="19">
         <v>1581.1512608850701</v>
       </c>
-      <c r="G24" s="24">
+      <c r="G24" s="17">
         <v>1.00130638837852</v>
       </c>
-      <c r="H24" s="23">
+      <c r="H24" s="16">
         <v>3.54109589041096E-3</v>
       </c>
       <c r="I24" s="6">
         <v>3.4157534246575298E-2</v>
       </c>
-      <c r="J24" s="25">
+      <c r="J24" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K24" s="25">
+      <c r="K24" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="24">
+      <c r="B25" s="17">
         <v>3.8214828202307798</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="17">
         <v>5.8777598168660097</v>
       </c>
       <c r="D25" s="6">
@@ -2236,30 +2113,30 @@
       <c r="E25" s="6">
         <v>3.7712328767123299E-2</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="19">
         <v>1601.1766776740601</v>
       </c>
-      <c r="G25" s="24">
+      <c r="G25" s="17">
         <v>1.00552699900417</v>
       </c>
-      <c r="H25" s="23">
+      <c r="H25" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I25" s="6">
         <v>3.42808219178082E-2</v>
       </c>
-      <c r="J25" s="25">
+      <c r="J25" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K25" s="25">
+      <c r="K25" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="24">
+      <c r="B26" s="17">
         <v>3.81238501772085</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="17">
         <v>6.1543550566573604</v>
       </c>
       <c r="D26" s="6">
@@ -2268,30 +2145,30 @@
       <c r="E26" s="6">
         <v>3.7732876712328799E-2</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="19">
         <v>1564.84793037144</v>
       </c>
-      <c r="G26" s="24">
+      <c r="G26" s="17">
         <v>1.0122942866478899</v>
       </c>
-      <c r="H26" s="23">
+      <c r="H26" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I26" s="6">
         <v>3.4219178082191798E-2</v>
       </c>
-      <c r="J26" s="25">
+      <c r="J26" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K26" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="24">
+      <c r="B27" s="17">
         <v>3.9326877561604801</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="17">
         <v>6.3485604591033802</v>
       </c>
       <c r="D27" s="6">
@@ -2300,30 +2177,30 @@
       <c r="E27" s="6">
         <v>3.7760273972602697E-2</v>
       </c>
-      <c r="F27" s="26">
+      <c r="F27" s="19">
         <v>1578.06568569465</v>
       </c>
-      <c r="G27" s="24">
+      <c r="G27" s="17">
         <v>1.0032642321983301</v>
       </c>
-      <c r="H27" s="23">
+      <c r="H27" s="16">
         <v>3.54109589041096E-3</v>
       </c>
       <c r="I27" s="6">
         <v>3.4219178082191798E-2</v>
       </c>
-      <c r="J27" s="25">
+      <c r="J27" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K27" s="25">
+      <c r="K27" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="24">
+      <c r="B28" s="17">
         <v>3.81462335764959</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="17">
         <v>5.8672093903897897</v>
       </c>
       <c r="D28" s="6">
@@ -2332,30 +2209,30 @@
       <c r="E28" s="6">
         <v>3.7773972602739701E-2</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F28" s="19">
         <v>1598.0721249897101</v>
       </c>
-      <c r="G28" s="24">
+      <c r="G28" s="17">
         <v>1.0074804224417799</v>
       </c>
-      <c r="H28" s="23">
+      <c r="H28" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I28" s="6">
         <v>3.43424657534247E-2</v>
       </c>
-      <c r="J28" s="25">
+      <c r="J28" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K28" s="25">
+      <c r="K28" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="24">
+      <c r="B29" s="17">
         <v>3.8055295801265401</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="17">
         <v>6.1432882843277001</v>
       </c>
       <c r="D29" s="6">
@@ -2364,30 +2241,30 @@
       <c r="E29" s="6">
         <v>3.7794520547945201E-2</v>
       </c>
-      <c r="F29" s="26">
+      <c r="F29" s="19">
         <v>1561.8020729365799</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="17">
         <v>1.0142684830794899</v>
       </c>
-      <c r="H29" s="23">
+      <c r="H29" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I29" s="6">
         <v>3.42808219178082E-2</v>
       </c>
-      <c r="J29" s="25">
+      <c r="J29" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K29" s="25">
+      <c r="K29" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="24">
+      <c r="B30" s="17">
         <v>3.9256159899655798</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="17">
         <v>6.3371444662698302</v>
       </c>
       <c r="D30" s="6">
@@ -2396,30 +2273,30 @@
       <c r="E30" s="6">
         <v>3.7821917808219203E-2</v>
       </c>
-      <c r="F30" s="26">
+      <c r="F30" s="19">
         <v>1574.9921290823099</v>
       </c>
-      <c r="G30" s="24">
+      <c r="G30" s="17">
         <v>1.00522207653155</v>
       </c>
-      <c r="H30" s="23">
+      <c r="H30" s="16">
         <v>3.54109589041096E-3</v>
       </c>
       <c r="I30" s="6">
         <v>3.42808219178082E-2</v>
       </c>
-      <c r="J30" s="25">
+      <c r="J30" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K30" s="25">
+      <c r="K30" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="24">
+      <c r="B31" s="17">
         <v>3.80778847606113</v>
       </c>
-      <c r="C31" s="24">
+      <c r="C31" s="17">
         <v>5.8566967715338301</v>
       </c>
       <c r="D31" s="6">
@@ -2428,30 +2305,30 @@
       <c r="E31" s="6">
         <v>3.7835616438356201E-2</v>
       </c>
-      <c r="F31" s="26">
+      <c r="F31" s="19">
         <v>1594.9795869884301</v>
       </c>
-      <c r="G31" s="24">
+      <c r="G31" s="17">
         <v>1.0094338464964501</v>
       </c>
-      <c r="H31" s="23">
+      <c r="H31" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I31" s="6">
         <v>3.4404109589041103E-2</v>
       </c>
-      <c r="J31" s="25">
+      <c r="J31" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K31" s="25">
+      <c r="K31" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="24">
+      <c r="B32" s="17">
         <v>3.9308586219878001</v>
       </c>
-      <c r="C32" s="24">
+      <c r="C32" s="17">
         <v>6.0459889370131803</v>
       </c>
       <c r="D32" s="6">
@@ -2460,30 +2337,30 @@
       <c r="E32" s="6">
         <v>3.7863013698630099E-2</v>
       </c>
-      <c r="F32" s="26">
+      <c r="F32" s="19">
         <v>1608.74198499463</v>
       </c>
-      <c r="G32" s="24">
+      <c r="G32" s="17">
         <v>1.00021719977891</v>
       </c>
-      <c r="H32" s="23">
+      <c r="H32" s="16">
         <v>3.4589041095890402E-3</v>
       </c>
       <c r="I32" s="6">
         <v>3.4404109589041103E-2</v>
       </c>
-      <c r="J32" s="25">
+      <c r="J32" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K32" s="25">
+      <c r="K32" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="24">
+      <c r="B33" s="17">
         <v>3.91856961104462</v>
       </c>
-      <c r="C33" s="24">
+      <c r="C33" s="17">
         <v>6.3257694562585698</v>
       </c>
       <c r="D33" s="6">
@@ -2492,30 +2369,30 @@
       <c r="E33" s="6">
         <v>3.7883561643835599E-2</v>
       </c>
-      <c r="F33" s="26">
+      <c r="F33" s="19">
         <v>1571.9305209564</v>
       </c>
-      <c r="G33" s="24">
+      <c r="G33" s="17">
         <v>1.0071799213833601</v>
       </c>
-      <c r="H33" s="23">
+      <c r="H33" s="16">
         <v>3.54109589041096E-3</v>
       </c>
       <c r="I33" s="6">
         <v>3.43424657534247E-2</v>
       </c>
-      <c r="J33" s="25">
+      <c r="J33" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K33" s="25">
+      <c r="K33" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="24">
+      <c r="B34" s="17">
         <v>3.8009780435721501</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C34" s="17">
         <v>5.8462217574353001</v>
       </c>
       <c r="D34" s="6">
@@ -2524,30 +2401,30 @@
       <c r="E34" s="6">
         <v>3.7897260273972597E-2</v>
       </c>
-      <c r="F34" s="26">
+      <c r="F34" s="19">
         <v>1591.89899405345</v>
       </c>
-      <c r="G34" s="24">
+      <c r="G34" s="17">
         <v>1.0113872711719301</v>
       </c>
-      <c r="H34" s="23">
+      <c r="H34" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I34" s="6">
         <v>3.4465753424657498E-2</v>
       </c>
-      <c r="J34" s="25">
+      <c r="J34" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K34" s="25">
+      <c r="K34" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="24">
+      <c r="B35" s="17">
         <v>3.8578383595086998</v>
       </c>
-      <c r="C35" s="24">
+      <c r="C35" s="17">
         <v>6.2277306476781398</v>
       </c>
       <c r="D35" s="6">
@@ -2556,30 +2433,30 @@
       <c r="E35" s="6">
         <v>3.7917808219178097E-2</v>
       </c>
-      <c r="F35" s="26">
+      <c r="F35" s="19">
         <v>1582.8022372876501</v>
       </c>
-      <c r="G35" s="24">
+      <c r="G35" s="17">
         <v>1.0008114608823999</v>
       </c>
-      <c r="H35" s="23">
+      <c r="H35" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I35" s="6">
         <v>3.4404109589041103E-2</v>
       </c>
-      <c r="J35" s="25">
+      <c r="J35" s="18">
         <v>3.1506849315068499</v>
       </c>
-      <c r="K35" s="25">
+      <c r="K35" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="24">
+      <c r="B36" s="17">
         <v>3.9238280719882201</v>
       </c>
-      <c r="C36" s="24">
+      <c r="C36" s="17">
         <v>6.0351753637951502</v>
       </c>
       <c r="D36" s="6">
@@ -2588,30 +2465,30 @@
       <c r="E36" s="6">
         <v>3.7924657534246599E-2</v>
       </c>
-      <c r="F36" s="26">
+      <c r="F36" s="19">
         <v>1605.6328322572401</v>
       </c>
-      <c r="G36" s="24">
+      <c r="G36" s="17">
         <v>1.0021540236792501</v>
       </c>
-      <c r="H36" s="23">
+      <c r="H36" s="16">
         <v>3.4589041095890402E-3</v>
       </c>
       <c r="I36" s="6">
         <v>3.4465753424657498E-2</v>
       </c>
-      <c r="J36" s="25">
+      <c r="J36" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K36" s="25">
+      <c r="K36" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="24">
+      <c r="B37" s="17">
         <v>3.9115484829340499</v>
       </c>
-      <c r="C37" s="24">
+      <c r="C37" s="17">
         <v>6.3144352087757296</v>
       </c>
       <c r="D37" s="6">
@@ -2620,30 +2497,30 @@
       <c r="E37" s="6">
         <v>3.7945205479452099E-2</v>
       </c>
-      <c r="F37" s="26">
+      <c r="F37" s="19">
         <v>1568.88079176939</v>
       </c>
-      <c r="G37" s="24">
+      <c r="G37" s="17">
         <v>1.0091377667588199</v>
       </c>
-      <c r="H37" s="23">
+      <c r="H37" s="16">
         <v>3.54109589041096E-3</v>
       </c>
       <c r="I37" s="6">
         <v>3.4404109589041103E-2</v>
       </c>
-      <c r="J37" s="25">
+      <c r="J37" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K37" s="25">
+      <c r="K37" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="24">
+      <c r="B38" s="17">
         <v>3.8641451834955398</v>
       </c>
-      <c r="C38" s="24">
+      <c r="C38" s="17">
         <v>5.7138671401851999</v>
       </c>
       <c r="D38" s="6">
@@ -2652,30 +2529,30 @@
       <c r="E38" s="6">
         <v>3.7965753424657502E-2</v>
       </c>
-      <c r="F38" s="26">
+      <c r="F38" s="19">
         <v>1630.30033093867</v>
       </c>
-      <c r="G38" s="24">
+      <c r="G38" s="17">
         <v>1.0012600843628501</v>
       </c>
-      <c r="H38" s="23">
+      <c r="H38" s="16">
         <v>3.3767123287671199E-3</v>
       </c>
       <c r="I38" s="6">
         <v>3.4589041095890401E-2</v>
       </c>
-      <c r="J38" s="25">
+      <c r="J38" s="18">
         <v>3.4246575342465801</v>
       </c>
-      <c r="K38" s="25">
+      <c r="K38" s="18">
         <v>62.671232876712303</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="24">
+      <c r="B39" s="17">
         <v>3.8509384101375601</v>
       </c>
-      <c r="C39" s="24">
+      <c r="C39" s="17">
         <v>6.2165920197311797</v>
       </c>
       <c r="D39" s="6">
@@ -2684,30 +2561,30 @@
       <c r="E39" s="6">
         <v>3.7979452054794499E-2</v>
       </c>
-      <c r="F39" s="26">
+      <c r="F39" s="19">
         <v>1579.7393158104801</v>
       </c>
-      <c r="G39" s="24">
+      <c r="G39" s="17">
         <v>1.00275191199826</v>
       </c>
-      <c r="H39" s="23">
+      <c r="H39" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I39" s="6">
         <v>3.4465753424657498E-2</v>
       </c>
-      <c r="J39" s="25">
+      <c r="J39" s="18">
         <v>3.1506849315068499</v>
       </c>
-      <c r="K39" s="25">
+      <c r="K39" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="24">
+      <c r="B40" s="17">
         <v>3.9168226261147998</v>
       </c>
-      <c r="C40" s="24">
+      <c r="C40" s="17">
         <v>6.0244004028203104</v>
       </c>
       <c r="D40" s="6">
@@ -2716,30 +2593,30 @@
       <c r="E40" s="6">
         <v>3.7986301369863001E-2</v>
       </c>
-      <c r="F40" s="26">
+      <c r="F40" s="19">
         <v>1602.5356732600601</v>
       </c>
-      <c r="G40" s="24">
+      <c r="G40" s="17">
         <v>1.0040908481773201</v>
       </c>
-      <c r="H40" s="23">
+      <c r="H40" s="16">
         <v>3.4589041095890402E-3</v>
       </c>
       <c r="I40" s="6">
         <v>3.4527397260273998E-2</v>
       </c>
-      <c r="J40" s="25">
+      <c r="J40" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K40" s="25">
+      <c r="K40" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="24">
+      <c r="B41" s="17">
         <v>3.9045524701466099</v>
       </c>
-      <c r="C41" s="24">
+      <c r="C41" s="17">
         <v>6.3031415051034401</v>
       </c>
       <c r="D41" s="6">
@@ -2748,30 +2625,30 @@
       <c r="E41" s="6">
         <v>3.8006849315068501E-2</v>
       </c>
-      <c r="F41" s="26">
+      <c r="F41" s="19">
         <v>1565.8428725126</v>
       </c>
-      <c r="G41" s="24">
+      <c r="G41" s="17">
         <v>1.0110956126629</v>
       </c>
-      <c r="H41" s="23">
+      <c r="H41" s="16">
         <v>3.54109589041096E-3</v>
       </c>
       <c r="I41" s="6">
         <v>3.4465753424657498E-2</v>
       </c>
-      <c r="J41" s="25">
+      <c r="J41" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K41" s="25">
+      <c r="K41" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="24">
+      <c r="B42" s="17">
         <v>3.8572708394252699</v>
       </c>
-      <c r="C42" s="24">
+      <c r="C42" s="17">
         <v>5.7037021264944201</v>
       </c>
       <c r="D42" s="6">
@@ -2780,30 +2657,30 @@
       <c r="E42" s="6">
         <v>3.8027397260274001E-2</v>
       </c>
-      <c r="F42" s="26">
+      <c r="F42" s="19">
         <v>1627.1736115991098</v>
       </c>
-      <c r="G42" s="24">
+      <c r="G42" s="17">
         <v>1.00318407037601</v>
       </c>
-      <c r="H42" s="23">
+      <c r="H42" s="16">
         <v>3.3767123287671199E-3</v>
       </c>
       <c r="I42" s="6">
         <v>3.4650684931506803E-2</v>
       </c>
-      <c r="J42" s="25">
+      <c r="J42" s="18">
         <v>3.4246575342465801</v>
       </c>
-      <c r="K42" s="25">
+      <c r="K42" s="18">
         <v>62.671232876712303</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="24">
+      <c r="B43" s="17">
         <v>3.8440630985542898</v>
       </c>
-      <c r="C43" s="24">
+      <c r="C43" s="17">
         <v>6.2054931647068603</v>
       </c>
       <c r="D43" s="6">
@@ -2812,30 +2689,30 @@
       <c r="E43" s="6">
         <v>3.8041095890410999E-2</v>
       </c>
-      <c r="F43" s="26">
+      <c r="F43" s="19">
         <v>1576.6882248469701</v>
       </c>
-      <c r="G43" s="24">
+      <c r="G43" s="17">
         <v>1.00469236366723</v>
       </c>
-      <c r="H43" s="23">
+      <c r="H43" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I43" s="6">
         <v>3.4527397260273998E-2</v>
       </c>
-      <c r="J43" s="25">
+      <c r="J43" s="18">
         <v>3.1506849315068499</v>
       </c>
-      <c r="K43" s="25">
+      <c r="K43" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="24">
+      <c r="B44" s="17">
         <v>3.9098421501474698</v>
       </c>
-      <c r="C44" s="24">
+      <c r="C44" s="17">
         <v>6.0136638476469697</v>
       </c>
       <c r="D44" s="6">
@@ -2844,30 +2721,30 @@
       <c r="E44" s="6">
         <v>3.8047945205479397E-2</v>
       </c>
-      <c r="F44" s="26">
+      <c r="F44" s="19">
         <v>1599.45043873074</v>
       </c>
-      <c r="G44" s="24">
+      <c r="G44" s="17">
         <v>1.00602767327696</v>
       </c>
-      <c r="H44" s="23">
+      <c r="H44" s="16">
         <v>3.4589041095890402E-3</v>
       </c>
       <c r="I44" s="6">
         <v>3.4589041095890401E-2</v>
       </c>
-      <c r="J44" s="25">
+      <c r="J44" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K44" s="25">
+      <c r="K44" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="24">
+      <c r="B45" s="17">
         <v>3.8975814381626201</v>
       </c>
-      <c r="C45" s="24">
+      <c r="C45" s="17">
         <v>6.2918881280857999</v>
       </c>
       <c r="D45" s="6">
@@ -2876,30 +2753,30 @@
       <c r="E45" s="6">
         <v>3.8068493150684897E-2</v>
       </c>
-      <c r="F45" s="26">
+      <c r="F45" s="19">
         <v>1562.8166947109899</v>
       </c>
-      <c r="G45" s="24">
+      <c r="G45" s="17">
         <v>1.0130534591005</v>
       </c>
-      <c r="H45" s="23">
+      <c r="H45" s="16">
         <v>3.54109589041096E-3</v>
       </c>
       <c r="I45" s="6">
         <v>3.4527397260273998E-2</v>
       </c>
-      <c r="J45" s="25">
+      <c r="J45" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K45" s="25">
+      <c r="K45" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="24">
+      <c r="B46" s="17">
         <v>3.8442331801479699</v>
       </c>
-      <c r="C46" s="24">
+      <c r="C46" s="17">
         <v>5.9127517709401198</v>
       </c>
       <c r="D46" s="6">
@@ -2908,30 +2785,30 @@
       <c r="E46" s="6">
         <v>3.8082191780821902E-2</v>
       </c>
-      <c r="F46" s="26">
+      <c r="F46" s="19">
         <v>1609.32867140903</v>
       </c>
-      <c r="G46" s="24">
+      <c r="G46" s="17">
         <v>1.0004335398855599</v>
       </c>
-      <c r="H46" s="23">
+      <c r="H46" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I46" s="6">
         <v>3.4650684931506803E-2</v>
       </c>
-      <c r="J46" s="25">
+      <c r="J46" s="18">
         <v>3.2602739726027399</v>
       </c>
-      <c r="K46" s="25">
+      <c r="K46" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="24">
+      <c r="B47" s="17">
         <v>3.85042091094168</v>
       </c>
-      <c r="C47" s="24">
+      <c r="C47" s="17">
         <v>5.6935732158514698</v>
       </c>
       <c r="D47" s="6">
@@ -2940,30 +2817,30 @@
       <c r="E47" s="6">
         <v>3.8089041095890397E-2</v>
       </c>
-      <c r="F47" s="26">
+      <c r="F47" s="19">
         <v>1624.0588615706101</v>
       </c>
-      <c r="G47" s="24">
+      <c r="G47" s="17">
         <v>1.00510805705269</v>
       </c>
-      <c r="H47" s="23">
+      <c r="H47" s="16">
         <v>3.3767123287671199E-3</v>
       </c>
       <c r="I47" s="6">
         <v>3.4712328767123303E-2</v>
       </c>
-      <c r="J47" s="25">
+      <c r="J47" s="18">
         <v>3.4246575342465801</v>
       </c>
-      <c r="K47" s="25">
+      <c r="K47" s="18">
         <v>62.671232876712303</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="24">
+      <c r="B48" s="17">
         <v>3.83721229303212</v>
       </c>
-      <c r="C48" s="24">
+      <c r="C48" s="17">
         <v>6.19443386995788</v>
       </c>
       <c r="D48" s="6">
@@ -2972,30 +2849,30 @@
       <c r="E48" s="6">
         <v>3.8102739726027401E-2</v>
       </c>
-      <c r="F48" s="26">
+      <c r="F48" s="19">
         <v>1573.6488959793799</v>
       </c>
-      <c r="G48" s="24">
+      <c r="G48" s="17">
         <v>1.0066328158937301</v>
       </c>
-      <c r="H48" s="23">
+      <c r="H48" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I48" s="6">
         <v>3.4589041095890401E-2</v>
       </c>
-      <c r="J48" s="25">
+      <c r="J48" s="18">
         <v>3.1506849315068499</v>
       </c>
-      <c r="K48" s="25">
+      <c r="K48" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="24">
+      <c r="B49" s="17">
         <v>3.9028865108212498</v>
       </c>
-      <c r="C49" s="24">
+      <c r="C49" s="17">
         <v>6.0029654933024696</v>
       </c>
       <c r="D49" s="6">
@@ -3004,30 +2881,30 @@
       <c r="E49" s="6">
         <v>3.8109589041095897E-2</v>
       </c>
-      <c r="F49" s="26">
+      <c r="F49" s="19">
         <v>1596.3770599295299</v>
       </c>
-      <c r="G49" s="24">
+      <c r="G49" s="17">
         <v>1.0079644989819201</v>
       </c>
-      <c r="H49" s="23">
+      <c r="H49" s="16">
         <v>3.4589041095890402E-3</v>
       </c>
       <c r="I49" s="6">
         <v>3.4650684931506803E-2</v>
       </c>
-      <c r="J49" s="25">
+      <c r="J49" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K49" s="25">
+      <c r="K49" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="24">
+      <c r="B50" s="17">
         <v>3.89063525342134</v>
       </c>
-      <c r="C50" s="24">
+      <c r="C50" s="17">
         <v>6.2806748621149504</v>
       </c>
       <c r="D50" s="6">
@@ -3036,30 +2913,30 @@
       <c r="E50" s="6">
         <v>3.8130136986301397E-2</v>
       </c>
-      <c r="F50" s="26">
+      <c r="F50" s="19">
         <v>1559.80219041798</v>
       </c>
-      <c r="G50" s="24">
+      <c r="G50" s="17">
         <v>1.0150113060763899</v>
       </c>
-      <c r="H50" s="23">
+      <c r="H50" s="16">
         <v>3.54109589041096E-3</v>
       </c>
       <c r="I50" s="6">
         <v>3.4589041095890401E-2</v>
       </c>
-      <c r="J50" s="25">
+      <c r="J50" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K50" s="25">
+      <c r="K50" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="24">
+      <c r="B51" s="17">
         <v>3.8374064045715399</v>
       </c>
-      <c r="C51" s="24">
+      <c r="C51" s="17">
         <v>5.9022516198078296</v>
       </c>
       <c r="D51" s="6">
@@ -3068,30 +2945,30 @@
       <c r="E51" s="6">
         <v>3.8143835616438401E-2</v>
       </c>
-      <c r="F51" s="26">
+      <c r="F51" s="19">
         <v>1606.2441900701799</v>
       </c>
-      <c r="G51" s="24">
+      <c r="G51" s="17">
         <v>1.00235467902718</v>
       </c>
-      <c r="H51" s="23">
+      <c r="H51" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I51" s="6">
         <v>3.4712328767123303E-2</v>
       </c>
-      <c r="J51" s="25">
+      <c r="J51" s="18">
         <v>3.2602739726027399</v>
       </c>
-      <c r="K51" s="25">
+      <c r="K51" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="24">
+      <c r="B52" s="17">
         <v>3.8435952682002101</v>
       </c>
-      <c r="C52" s="24">
+      <c r="C52" s="17">
         <v>5.6834802162567</v>
       </c>
       <c r="D52" s="6">
@@ -3100,30 +2977,30 @@
       <c r="E52" s="6">
         <v>3.8150684931506897E-2</v>
       </c>
-      <c r="F52" s="26">
+      <c r="F52" s="19">
         <v>1620.9560122508799</v>
       </c>
-      <c r="G52" s="24">
+      <c r="G52" s="17">
         <v>1.00703204439566</v>
       </c>
-      <c r="H52" s="23">
+      <c r="H52" s="16">
         <v>3.3767123287671199E-3</v>
       </c>
       <c r="I52" s="6">
         <v>3.4773972602739699E-2</v>
       </c>
-      <c r="J52" s="25">
+      <c r="J52" s="18">
         <v>3.4246575342465801</v>
       </c>
-      <c r="K52" s="25">
+      <c r="K52" s="18">
         <v>62.671232876712303</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="24">
+      <c r="B53" s="17">
         <v>3.8303858627816099</v>
       </c>
-      <c r="C53" s="24">
+      <c r="C53" s="17">
         <v>6.1834139243501198</v>
       </c>
       <c r="D53" s="6">
@@ -3132,30 +3009,30 @@
       <c r="E53" s="6">
         <v>3.8164383561643797E-2</v>
       </c>
-      <c r="F53" s="26">
+      <c r="F53" s="19">
         <v>1570.6212613166499</v>
       </c>
-      <c r="G53" s="24">
+      <c r="G53" s="17">
         <v>1.00857326868213</v>
       </c>
-      <c r="H53" s="23">
+      <c r="H53" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I53" s="6">
         <v>3.4650684931506803E-2</v>
       </c>
-      <c r="J53" s="25">
+      <c r="J53" s="18">
         <v>3.1506849315068499</v>
       </c>
-      <c r="K53" s="25">
+      <c r="K53" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="24">
+      <c r="B54" s="17">
         <v>3.8959555758178199</v>
       </c>
-      <c r="C54" s="24">
+      <c r="C54" s="17">
         <v>5.9923051362701596</v>
       </c>
       <c r="D54" s="6">
@@ -3164,30 +3041,30 @@
       <c r="E54" s="6">
         <v>3.8171232876712299E-2</v>
       </c>
-      <c r="F54" s="26">
+      <c r="F54" s="19">
         <v>1593.3154686440998</v>
       </c>
-      <c r="G54" s="24">
+      <c r="G54" s="17">
         <v>1.0099013252958799</v>
       </c>
-      <c r="H54" s="23">
+      <c r="H54" s="16">
         <v>3.4589041095890402E-3</v>
       </c>
       <c r="I54" s="6">
         <v>3.4712328767123303E-2</v>
       </c>
-      <c r="J54" s="25">
+      <c r="J54" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K54" s="25">
+      <c r="K54" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="24">
+      <c r="B55" s="17">
         <v>3.88371378331246</v>
       </c>
-      <c r="C55" s="24">
+      <c r="C55" s="17">
         <v>6.2695014931173203</v>
       </c>
       <c r="D55" s="6">
@@ -3196,30 +3073,30 @@
       <c r="E55" s="6">
         <v>3.8191780821917799E-2</v>
       </c>
-      <c r="F55" s="26">
+      <c r="F55" s="19">
         <v>1556.7992922104199</v>
       </c>
-      <c r="G55" s="24">
+      <c r="G55" s="17">
         <v>1.0169691535952901</v>
       </c>
-      <c r="H55" s="23">
+      <c r="H55" s="16">
         <v>3.54109589041096E-3</v>
       </c>
       <c r="I55" s="6">
         <v>3.4650684931506803E-2</v>
       </c>
-      <c r="J55" s="25">
+      <c r="J55" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K55" s="25">
+      <c r="K55" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="24">
+      <c r="B56" s="17">
         <v>3.83060383265089</v>
       </c>
-      <c r="C56" s="24">
+      <c r="C56" s="17">
         <v>5.8917886959200496</v>
       </c>
       <c r="D56" s="6">
@@ -3228,30 +3105,30 @@
       <c r="E56" s="6">
         <v>3.8205479452054797E-2</v>
       </c>
-      <c r="F56" s="26">
+      <c r="F56" s="19">
         <v>1603.17150870606</v>
       </c>
-      <c r="G56" s="24">
+      <c r="G56" s="17">
         <v>1.0042758187965399</v>
       </c>
-      <c r="H56" s="23">
+      <c r="H56" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I56" s="6">
         <v>3.4773972602739699E-2</v>
       </c>
-      <c r="J56" s="25">
+      <c r="J56" s="18">
         <v>3.2602739726027399</v>
       </c>
-      <c r="K56" s="25">
+      <c r="K56" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="24">
+      <c r="B57" s="17">
         <v>3.83679378227535</v>
       </c>
-      <c r="C57" s="24">
+      <c r="C57" s="17">
         <v>5.6734229370694598</v>
       </c>
       <c r="D57" s="6">
@@ -3260,30 +3137,30 @@
       <c r="E57" s="6">
         <v>3.8212328767123299E-2</v>
       </c>
-      <c r="F57" s="26">
+      <c r="F57" s="19">
         <v>1617.8649955610399</v>
       </c>
-      <c r="G57" s="24">
+      <c r="G57" s="17">
         <v>1.0089560324076201</v>
       </c>
-      <c r="H57" s="23">
+      <c r="H57" s="16">
         <v>3.3767123287671199E-3</v>
       </c>
       <c r="I57" s="6">
         <v>3.4835616438356198E-2</v>
       </c>
-      <c r="J57" s="25">
+      <c r="J57" s="18">
         <v>3.4246575342465801</v>
       </c>
-      <c r="K57" s="25">
+      <c r="K57" s="18">
         <v>62.671232876712303</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="24">
+      <c r="B58" s="17">
         <v>3.8235836779424202</v>
       </c>
-      <c r="C58" s="24">
+      <c r="C58" s="17">
         <v>6.17243311824926</v>
       </c>
       <c r="D58" s="6">
@@ -3292,30 +3169,30 @@
       <c r="E58" s="6">
         <v>3.8226027397260297E-2</v>
       </c>
-      <c r="F58" s="26">
+      <c r="F58" s="19">
         <v>1567.6052534893502</v>
       </c>
-      <c r="G58" s="24">
+      <c r="G58" s="17">
         <v>1.01051372203668</v>
       </c>
-      <c r="H58" s="23">
+      <c r="H58" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I58" s="6">
         <v>3.4712328767123303E-2</v>
       </c>
-      <c r="J58" s="25">
+      <c r="J58" s="18">
         <v>3.1506849315068499</v>
       </c>
-      <c r="K58" s="25">
+      <c r="K58" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="24">
+      <c r="B59" s="17">
         <v>3.8890492137570898</v>
       </c>
-      <c r="C59" s="24">
+      <c r="C59" s="17">
         <v>5.9816825744765003</v>
       </c>
       <c r="D59" s="6">
@@ -3324,30 +3201,30 @@
       <c r="E59" s="6">
         <v>3.8232876712328799E-2</v>
       </c>
-      <c r="F59" s="26">
+      <c r="F59" s="19">
         <v>1590.26559718454</v>
       </c>
-      <c r="G59" s="24">
+      <c r="G59" s="17">
         <v>1.01183815222243</v>
       </c>
-      <c r="H59" s="23">
+      <c r="H59" s="16">
         <v>3.4589041095890402E-3</v>
       </c>
       <c r="I59" s="6">
         <v>3.4773972602739699E-2</v>
       </c>
-      <c r="J59" s="25">
+      <c r="J59" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K59" s="25">
+      <c r="K59" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="24">
+      <c r="B60" s="17">
         <v>3.9442397987097202</v>
       </c>
-      <c r="C60" s="24">
+      <c r="C60" s="17">
         <v>6.36720898781891</v>
       </c>
       <c r="D60" s="6">
@@ -3356,30 +3233,30 @@
       <c r="E60" s="6">
         <v>3.8253424657534299E-2</v>
       </c>
-      <c r="F60" s="26">
+      <c r="F60" s="19">
         <v>1580.8306798475498</v>
       </c>
-      <c r="G60" s="24">
+      <c r="G60" s="17">
         <v>1.00150944607784</v>
       </c>
-      <c r="H60" s="23">
+      <c r="H60" s="16">
         <v>3.54109589041096E-3</v>
       </c>
       <c r="I60" s="6">
         <v>3.4712328767123303E-2</v>
       </c>
-      <c r="J60" s="25">
+      <c r="J60" s="18">
         <v>3.1506849315068499</v>
       </c>
-      <c r="K60" s="25">
+      <c r="K60" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B61" s="24">
+      <c r="B61" s="17">
         <v>3.8768168961676701</v>
       </c>
-      <c r="C61" s="24">
+      <c r="C61" s="17">
         <v>6.2583678085399601</v>
       </c>
       <c r="D61" s="6">
@@ -3388,30 +3265,30 @@
       <c r="E61" s="6">
         <v>3.8253424657534299E-2</v>
       </c>
-      <c r="F61" s="26">
+      <c r="F61" s="19">
         <v>1553.8079331834901</v>
       </c>
-      <c r="G61" s="24">
+      <c r="G61" s="17">
         <v>1.0189270016617999</v>
       </c>
-      <c r="H61" s="23">
+      <c r="H61" s="16">
         <v>3.54109589041096E-3</v>
       </c>
       <c r="I61" s="6">
         <v>3.4712328767123303E-2</v>
       </c>
-      <c r="J61" s="25">
+      <c r="J61" s="18">
         <v>3.20547945205479</v>
       </c>
-      <c r="K61" s="25">
+      <c r="K61" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="24">
+      <c r="B62" s="17">
         <v>3.8238253358962999</v>
       </c>
-      <c r="C62" s="24">
+      <c r="C62" s="17">
         <v>5.8813628016488604</v>
       </c>
       <c r="D62" s="6">
@@ -3420,30 +3297,30 @@
       <c r="E62" s="6">
         <v>3.8267123287671199E-2</v>
       </c>
-      <c r="F62" s="26">
+      <c r="F62" s="19">
         <v>1600.11055972794</v>
       </c>
-      <c r="G62" s="24">
+      <c r="G62" s="17">
         <v>1.00619695919688</v>
       </c>
-      <c r="H62" s="23">
+      <c r="H62" s="16">
         <v>3.4315068493150701E-3</v>
       </c>
       <c r="I62" s="6">
         <v>3.4835616438356198E-2</v>
       </c>
-      <c r="J62" s="25">
+      <c r="J62" s="18">
         <v>3.2602739726027399</v>
       </c>
-      <c r="K62" s="25">
+      <c r="K62" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="24">
+      <c r="B63" s="17">
         <v>3.8300163251525898</v>
       </c>
-      <c r="C63" s="24">
+      <c r="C63" s="17">
         <v>5.6634011889961302</v>
       </c>
       <c r="D63" s="6">
@@ -3452,30 +3329,30 @@
       <c r="E63" s="6">
         <v>3.8273972602739702E-2</v>
       </c>
-      <c r="F63" s="26">
+      <c r="F63" s="19">
         <v>1614.7857439405702</v>
       </c>
-      <c r="G63" s="24">
+      <c r="G63" s="17">
         <v>1.0108800210912201</v>
       </c>
-      <c r="H63" s="23">
+      <c r="H63" s="16">
         <v>3.3767123287671199E-3</v>
       </c>
       <c r="I63" s="6">
         <v>3.4897260273972601E-2</v>
       </c>
-      <c r="J63" s="25">
+      <c r="J63" s="18">
         <v>3.4246575342465801</v>
       </c>
-      <c r="K63" s="25">
+      <c r="K63" s="18">
         <v>62.671232876712303</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="24">
+      <c r="B64" s="17">
         <v>3.8168056095749798</v>
       </c>
-      <c r="C64" s="24">
+      <c r="C64" s="17">
         <v>6.1614912435074398</v>
       </c>
       <c r="D64" s="6">
@@ -3484,30 +3361,30 @@
       <c r="E64" s="6">
         <v>3.8287671232876699E-2</v>
       </c>
-      <c r="F64" s="26">
+      <c r="F64" s="19">
         <v>1564.6008056446499</v>
       </c>
-      <c r="G64" s="24">
+      <c r="G64" s="17">
         <v>1.0124541759615799</v>
       </c>
-      <c r="H64" s="23">
+      <c r="H64" s="16">
         <v>3.5136986301369899E-3</v>
       </c>
       <c r="I64" s="6">
         <v>3.4773972602739699E-2</v>
       </c>
-      <c r="J64" s="25">
+      <c r="J64" s="18">
         <v>3.1506849315068499</v>
       </c>
-      <c r="K64" s="25">
+      <c r="K64" s="18">
         <v>48.835616438356197</v>
       </c>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B65" s="24">
+      <c r="B65" s="17">
         <v>3.8821672941888998</v>
       </c>
-      <c r="C65" s="24">
+      <c r="C65" s="17">
         <v>5.9710976072782502</v>
       </c>
       <c r="D65" s="6">
@@ -3516,22 +3393,22 @@
       <c r="E65" s="6">
         <v>3.8294520547945202E-2</v>
       </c>
-      <c r="F65" s="26">
+      <c r="F65" s="19">
         <v>1587.2273783783301</v>
       </c>
-      <c r="G65" s="24">
+      <c r="G65" s="17">
         <v>1.0137749797650999</v>
       </c>
-      <c r="H65" s="23">
+      <c r="H65" s="16">
         <v>3.4589041095890402E-3</v>
       </c>
       <c r="I65" s="6">
         <v>3.4835616438356198E-2</v>
       </c>
-      <c r="J65" s="25">
+      <c r="J65" s="18">
         <v>3.3150684931506902</v>
       </c>
-      <c r="K65" s="25">
+      <c r="K65" s="18">
         <v>55.753424657534303</v>
       </c>
     </row>
@@ -3554,4 +3431,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>5.5</v>
+      </c>
+      <c r="D7">
+        <v>2.9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>8.25</v>
+      </c>
+      <c r="D8">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>2.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
A few performance tweaks and some changes to name-value pairs to allow a faster default run.
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="discrete_output" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$B$4:$H$18</definedName>
@@ -44,7 +45,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="##0.00E+0"/>
-    <numFmt numFmtId="166" formatCode="##0E+0"/>
+    <numFmt numFmtId="165" formatCode="##0E+0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -133,7 +134,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -443,7 +444,7 @@
   <dimension ref="B1:K104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1627,4 +1628,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>